<commit_message>
detailed scores par direction
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5F92C7-9B62-4562-B19C-947075E9356D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA1B21D-6708-43C7-978C-06F7F6B57A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Glenoid</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Total shear forces on the glenoid [N]</t>
+  </si>
+  <si>
+    <t>Total moment AP on the glenoid [N.m]</t>
+  </si>
+  <si>
+    <t>Total moment IS on the glenoid [N.m]</t>
+  </si>
+  <si>
+    <t>Total AP shear forces on the glenoid [N]</t>
+  </si>
+  <si>
+    <t>Total IS shear forces on the glenoid [N]</t>
   </si>
 </sst>
 </file>
@@ -210,16 +222,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -239,7 +248,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -250,6 +259,18 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -272,16 +293,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>539462</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>126651</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>177512</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>110199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -312,8 +333,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5391150" y="0"/>
-          <a:ext cx="8782050" cy="4489101"/>
+          <a:off x="11553826" y="0"/>
+          <a:ext cx="8782050" cy="4578290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,16 +345,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>690996</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>49790</xdr:rowOff>
+      <xdr:rowOff>67108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>73</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>729096</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>54985</xdr:rowOff>
+      <xdr:rowOff>30739</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -364,8 +385,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5819775" y="4602740"/>
-          <a:ext cx="50330100" cy="7625195"/>
+          <a:off x="12467360" y="4812290"/>
+          <a:ext cx="50330100" cy="7704858"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -694,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E3FA34-2DBA-4A8A-BF5F-CD7F590C191F}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,18 +729,26 @@
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+    </row>
+    <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -728,10 +757,20 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="F2" s="4"/>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -746,142 +785,276 @@
       <c r="E3" s="1">
         <v>7.85</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="H3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="M3" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
+        <v>182.73604698252799</v>
+      </c>
+      <c r="C4" s="9">
+        <v>169.965116238218</v>
+      </c>
+      <c r="D4" s="9">
+        <v>209.00959847145299</v>
+      </c>
+      <c r="E4" s="9">
+        <v>249.87519780755699</v>
+      </c>
+      <c r="F4" s="10">
+        <v>273.69375085206502</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="9">
         <v>3094.8796477168598</v>
       </c>
-      <c r="C4" s="10">
+      <c r="J4" s="9">
         <v>2992.8972374032401</v>
       </c>
-      <c r="D4" s="10">
+      <c r="K4" s="9">
         <v>3695.8390605910899</v>
       </c>
-      <c r="E4" s="10">
+      <c r="L4" s="9">
         <v>4418.3455812754501</v>
       </c>
-      <c r="F4" s="11">
+      <c r="M4" s="10">
         <v>4834.8187391920301</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
+        <v>179.827394726748</v>
+      </c>
+      <c r="C5" s="9">
+        <v>145.31407814489799</v>
+      </c>
+      <c r="D5" s="9">
+        <v>190.120758225305</v>
+      </c>
+      <c r="E5" s="9">
+        <v>250.31642299382401</v>
+      </c>
+      <c r="F5" s="10">
+        <v>276.630711232397</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="9">
         <v>3062.6578868668398</v>
       </c>
-      <c r="C5" s="10">
+      <c r="J5" s="9">
         <v>2442.3597758405299</v>
       </c>
-      <c r="D5" s="10">
+      <c r="K5" s="9">
         <v>3361.3836192029999</v>
       </c>
-      <c r="E5" s="10">
+      <c r="L5" s="9">
         <v>4424.1664384715596</v>
       </c>
-      <c r="F5" s="11">
+      <c r="M5" s="10">
         <v>4880.5017747422498</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
+        <v>195.04023456458799</v>
+      </c>
+      <c r="C6" s="9">
+        <v>141.26001699182299</v>
+      </c>
+      <c r="D6" s="9">
+        <v>175.327907172306</v>
+      </c>
+      <c r="E6" s="9">
+        <v>255.16060531322501</v>
+      </c>
+      <c r="F6" s="10">
+        <v>283.65502062246401</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="9">
         <v>3338.4983711975701</v>
       </c>
-      <c r="C6" s="10">
+      <c r="J6" s="9">
         <v>2382.3632449277102</v>
       </c>
-      <c r="D6" s="10">
+      <c r="K6" s="9">
         <v>3094.1893257229699</v>
       </c>
-      <c r="E6" s="10">
+      <c r="L6" s="9">
         <v>4506.0088455752702</v>
       </c>
-      <c r="F6" s="11">
+      <c r="M6" s="10">
         <v>4995.5384970136602</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
+        <v>218.01985016285201</v>
+      </c>
+      <c r="C7" s="9">
+        <v>144.98494010669</v>
+      </c>
+      <c r="D7" s="9">
+        <v>159.20782247769901</v>
+      </c>
+      <c r="E7" s="9">
+        <v>261.26579960812899</v>
+      </c>
+      <c r="F7" s="10">
+        <v>292.72806844669901</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="9">
         <v>3749.3313662270102</v>
       </c>
-      <c r="C7" s="10">
+      <c r="J7" s="9">
         <v>2459.75992369704</v>
       </c>
-      <c r="D7" s="10">
+      <c r="K7" s="9">
         <v>2766.9751053119198</v>
       </c>
-      <c r="E7" s="10">
+      <c r="L7" s="9">
         <v>4609.2774333979196</v>
       </c>
-      <c r="F7" s="11">
+      <c r="M7" s="10">
         <v>5140.2667193444504</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
+        <v>265.192655890808</v>
+      </c>
+      <c r="C8" s="9">
+        <v>171.32957880330599</v>
+      </c>
+      <c r="D8" s="9">
+        <v>161.342385017754</v>
+      </c>
+      <c r="E8" s="9">
+        <v>272.90885431698803</v>
+      </c>
+      <c r="F8" s="10">
+        <v>368.68107850545903</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="9">
         <v>4587.2809351962296</v>
       </c>
-      <c r="C8" s="10">
+      <c r="J8" s="9">
         <v>2939.7775350970301</v>
       </c>
-      <c r="D8" s="10">
+      <c r="K8" s="9">
         <v>2726.2602252619899</v>
       </c>
-      <c r="E8" s="10">
+      <c r="L8" s="9">
         <v>4806.6538656575703</v>
       </c>
-      <c r="F8" s="11">
+      <c r="M8" s="10">
         <v>5075.2425786429103</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
+        <v>278.60638039876397</v>
+      </c>
+      <c r="C9" s="11">
+        <v>200.27884649179001</v>
+      </c>
+      <c r="D9" s="11">
+        <v>192.66514587292201</v>
+      </c>
+      <c r="E9" s="11">
+        <v>295.41908599617301</v>
+      </c>
+      <c r="F9" s="12">
+        <v>388.59391117002099</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="11">
         <v>4831.28558021957</v>
       </c>
-      <c r="C9" s="12">
+      <c r="J9" s="11">
         <v>3458.00814326102</v>
       </c>
-      <c r="D9" s="12">
+      <c r="K9" s="11">
         <v>3290.29537868836</v>
       </c>
-      <c r="E9" s="12">
+      <c r="L9" s="11">
         <v>5192.5688422368403</v>
       </c>
-      <c r="F9" s="13">
+      <c r="M9" s="12">
         <v>5517.9643903629003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="11" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="H11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -890,10 +1063,20 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="F12" s="4"/>
+      <c r="H12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="1">
@@ -908,138 +1091,624 @@
       <c r="E13" s="1">
         <v>7.85</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="H13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="M13" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="10">
-        <v>182.73604698252799</v>
-      </c>
-      <c r="C14" s="10">
-        <v>169.965116238218</v>
-      </c>
-      <c r="D14" s="10">
-        <v>209.00959847145299</v>
-      </c>
-      <c r="E14" s="10">
-        <v>249.87519780755699</v>
-      </c>
-      <c r="F14" s="11">
-        <v>273.69375085206502</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="B14" s="9">
+        <v>121.059447796282</v>
+      </c>
+      <c r="C14" s="9">
+        <v>116.906198383478</v>
+      </c>
+      <c r="D14" s="9">
+        <v>137.85758780701801</v>
+      </c>
+      <c r="E14" s="9">
+        <v>162.691185062415</v>
+      </c>
+      <c r="F14" s="10">
+        <v>174.363445926016</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="9">
+        <v>994.33715279148305</v>
+      </c>
+      <c r="J14" s="9">
+        <v>962.57395308446496</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1302.2236597147</v>
+      </c>
+      <c r="L14" s="9">
+        <v>1595.48750433234</v>
+      </c>
+      <c r="M14" s="10">
+        <v>1811.6474802733101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="10">
-        <v>179.827394726748</v>
-      </c>
-      <c r="C15" s="10">
-        <v>145.31407814489799</v>
-      </c>
-      <c r="D15" s="10">
-        <v>190.120758225305</v>
-      </c>
-      <c r="E15" s="10">
-        <v>250.31642299382401</v>
-      </c>
-      <c r="F15" s="11">
-        <v>276.630711232397</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="B15" s="9">
+        <v>103.94718076968</v>
+      </c>
+      <c r="C15" s="9">
+        <v>91.068321671400298</v>
+      </c>
+      <c r="D15" s="9">
+        <v>132.48928413831001</v>
+      </c>
+      <c r="E15" s="9">
+        <v>170.65693738371499</v>
+      </c>
+      <c r="F15" s="10">
+        <v>182.31319746347401</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="9">
+        <v>1257.03723291285</v>
+      </c>
+      <c r="J15" s="9">
+        <v>858.531310508243</v>
+      </c>
+      <c r="K15" s="9">
+        <v>1058.4177612937301</v>
+      </c>
+      <c r="L15" s="9">
+        <v>1460.6758439601399</v>
+      </c>
+      <c r="M15" s="10">
+        <v>1719.33721034884</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10">
-        <v>195.04023456458799</v>
-      </c>
-      <c r="C16" s="10">
-        <v>141.26001699182299</v>
-      </c>
-      <c r="D16" s="10">
-        <v>175.327907172306</v>
-      </c>
-      <c r="E16" s="10">
-        <v>255.16060531322501</v>
-      </c>
-      <c r="F16" s="11">
-        <v>283.65502062246401</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="B16" s="9">
+        <v>105.164634240624</v>
+      </c>
+      <c r="C16" s="9">
+        <v>76.0574092633031</v>
+      </c>
+      <c r="D16" s="9">
+        <v>126.592080341298</v>
+      </c>
+      <c r="E16" s="9">
+        <v>178.35476995450901</v>
+      </c>
+      <c r="F16" s="10">
+        <v>190.69904866028401</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="9">
+        <v>1510.9825401404601</v>
+      </c>
+      <c r="J16" s="9">
+        <v>1059.1065756126</v>
+      </c>
+      <c r="K16" s="9">
+        <v>893.15748582663798</v>
+      </c>
+      <c r="L16" s="9">
+        <v>1408.3523546802801</v>
+      </c>
+      <c r="M16" s="10">
+        <v>1691.4302971130601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="10">
-        <v>218.01985016285201</v>
-      </c>
-      <c r="C17" s="10">
-        <v>144.98494010669</v>
-      </c>
-      <c r="D17" s="10">
-        <v>159.20782247769901</v>
-      </c>
-      <c r="E17" s="10">
-        <v>261.26579960812899</v>
-      </c>
-      <c r="F17" s="11">
-        <v>292.72806844669901</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="B17" s="9">
+        <v>110.895321691419</v>
+      </c>
+      <c r="C17" s="9">
+        <v>64.468866028476796</v>
+      </c>
+      <c r="D17" s="9">
+        <v>116.521812872198</v>
+      </c>
+      <c r="E17" s="9">
+        <v>186.82954582293999</v>
+      </c>
+      <c r="F17" s="10">
+        <v>200.52271762996199</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="9">
+        <v>1821.7007652494599</v>
+      </c>
+      <c r="J17" s="9">
+        <v>1337.72291048804</v>
+      </c>
+      <c r="K17" s="9">
+        <v>740.528852051493</v>
+      </c>
+      <c r="L17" s="9">
+        <v>1364.3759857366499</v>
+      </c>
+      <c r="M17" s="10">
+        <v>1671.8155325970999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="10">
-        <v>265.192655890808</v>
-      </c>
-      <c r="C18" s="10">
-        <v>171.32957880330599</v>
-      </c>
-      <c r="D18" s="10">
-        <v>161.342385017754</v>
-      </c>
-      <c r="E18" s="10">
-        <v>272.90885431698803</v>
-      </c>
-      <c r="F18" s="11">
-        <v>368.68107850545903</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="B18" s="9">
+        <v>121.063458344634</v>
+      </c>
+      <c r="C18" s="9">
+        <v>55.708866534578902</v>
+      </c>
+      <c r="D18" s="9">
+        <v>93.436026116025005</v>
+      </c>
+      <c r="E18" s="9">
+        <v>204.65569135918599</v>
+      </c>
+      <c r="F18" s="10">
+        <v>236.61450822179299</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="9">
+        <v>2482.3308587442798</v>
+      </c>
+      <c r="J18" s="9">
+        <v>1969.7857298045101</v>
+      </c>
+      <c r="K18" s="9">
+        <v>1100.6106568683899</v>
+      </c>
+      <c r="L18" s="9">
+        <v>1251.0702352478199</v>
+      </c>
+      <c r="M18" s="10">
+        <v>1163.1522427815</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="12">
-        <v>278.60638039876397</v>
-      </c>
-      <c r="C19" s="12">
-        <v>200.27884649179001</v>
-      </c>
-      <c r="D19" s="12">
-        <v>192.66514587292201</v>
-      </c>
-      <c r="E19" s="12">
-        <v>295.41908599617301</v>
-      </c>
-      <c r="F19" s="13">
-        <v>388.59391117002099</v>
+      <c r="B19" s="11">
+        <v>105.653555112183</v>
+      </c>
+      <c r="C19" s="11">
+        <v>53.066867532102101</v>
+      </c>
+      <c r="D19" s="11">
+        <v>97.197473959835605</v>
+      </c>
+      <c r="E19" s="11">
+        <v>235.43147693332199</v>
+      </c>
+      <c r="F19" s="12">
+        <v>289.88520078182</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="11">
+        <v>2993.1963695955101</v>
+      </c>
+      <c r="J19" s="11">
+        <v>2533.30879911078</v>
+      </c>
+      <c r="K19" s="11">
+        <v>1598.0874955036099</v>
+      </c>
+      <c r="L19" s="11">
+        <v>1099.1290604656799</v>
+      </c>
+      <c r="M19" s="12">
+        <v>1737.07657197458</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="H21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="H22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="F23" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="M23" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="9">
+        <v>61.676599186245298</v>
+      </c>
+      <c r="C24" s="9">
+        <v>53.058917854739299</v>
+      </c>
+      <c r="D24" s="9">
+        <v>71.152010664434698</v>
+      </c>
+      <c r="E24" s="9">
+        <v>87.184012745141999</v>
+      </c>
+      <c r="F24" s="10">
+        <v>99.330304926048697</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="9">
+        <v>2100.5424949253802</v>
+      </c>
+      <c r="J24" s="9">
+        <v>2030.32328431878</v>
+      </c>
+      <c r="K24" s="9">
+        <v>2393.6154008763901</v>
+      </c>
+      <c r="L24" s="9">
+        <v>2822.8580769431101</v>
+      </c>
+      <c r="M24" s="10">
+        <v>3023.17125891871</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="9">
+        <v>75.880213957067696</v>
+      </c>
+      <c r="C25" s="9">
+        <v>54.245756473498602</v>
+      </c>
+      <c r="D25" s="9">
+        <v>57.631474086994103</v>
+      </c>
+      <c r="E25" s="9">
+        <v>79.659485610109101</v>
+      </c>
+      <c r="F25" s="10">
+        <v>94.317513768922794</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="9">
+        <v>1805.6206539539901</v>
+      </c>
+      <c r="J25" s="9">
+        <v>1583.8284653322901</v>
+      </c>
+      <c r="K25" s="9">
+        <v>2302.9658579092702</v>
+      </c>
+      <c r="L25" s="9">
+        <v>2963.4905945114201</v>
+      </c>
+      <c r="M25" s="10">
+        <v>3161.1645643934098</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="9">
+        <v>89.875600323964406</v>
+      </c>
+      <c r="C26" s="9">
+        <v>65.202607728519993</v>
+      </c>
+      <c r="D26" s="9">
+        <v>48.735826831007202</v>
+      </c>
+      <c r="E26" s="9">
+        <v>76.805835358716095</v>
+      </c>
+      <c r="F26" s="10">
+        <v>92.9559719621802</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="9">
+        <v>1827.5158310571001</v>
+      </c>
+      <c r="J26" s="9">
+        <v>1323.25666931511</v>
+      </c>
+      <c r="K26" s="9">
+        <v>2201.03183989633</v>
+      </c>
+      <c r="L26" s="9">
+        <v>3097.6564908949799</v>
+      </c>
+      <c r="M26" s="10">
+        <v>3304.1081999006001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="9">
+        <v>107.124528471432</v>
+      </c>
+      <c r="C27" s="9">
+        <v>80.516074078213506</v>
+      </c>
+      <c r="D27" s="9">
+        <v>42.686009605500601</v>
+      </c>
+      <c r="E27" s="9">
+        <v>74.436253785188597</v>
+      </c>
+      <c r="F27" s="10">
+        <v>92.205350816736697</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1927.6306009775501</v>
+      </c>
+      <c r="J27" s="9">
+        <v>1122.0370132089899</v>
+      </c>
+      <c r="K27" s="9">
+        <v>2026.44625326043</v>
+      </c>
+      <c r="L27" s="9">
+        <v>3244.9014476612601</v>
+      </c>
+      <c r="M27" s="10">
+        <v>3468.4511867473402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="9">
+        <v>144.129197546174</v>
+      </c>
+      <c r="C28" s="9">
+        <v>115.620712268727</v>
+      </c>
+      <c r="D28" s="9">
+        <v>67.906358901729007</v>
+      </c>
+      <c r="E28" s="9">
+        <v>68.253162957802004</v>
+      </c>
+      <c r="F28" s="10">
+        <v>132.06657028366601</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="9">
+        <v>2104.9500764519498</v>
+      </c>
+      <c r="J28" s="9">
+        <v>969.99180529251896</v>
+      </c>
+      <c r="K28" s="9">
+        <v>1625.6495683936</v>
+      </c>
+      <c r="L28" s="9">
+        <v>3555.5836304097502</v>
+      </c>
+      <c r="M28" s="10">
+        <v>3912.0903358614</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="11">
+        <v>172.952825286581</v>
+      </c>
+      <c r="C29" s="11">
+        <v>147.211978959688</v>
+      </c>
+      <c r="D29" s="11">
+        <v>95.467671913086804</v>
+      </c>
+      <c r="E29" s="11">
+        <v>59.987609062850197</v>
+      </c>
+      <c r="F29" s="12">
+        <v>98.708710388200302</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I29" s="11">
+        <v>1838.0892106240599</v>
+      </c>
+      <c r="J29" s="11">
+        <v>924.69934415024397</v>
+      </c>
+      <c r="K29" s="11">
+        <v>1692.20788318474</v>
+      </c>
+      <c r="L29" s="11">
+        <v>4093.4397817711501</v>
+      </c>
+      <c r="M29" s="12">
+        <v>3780.8878183883198</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:F2"/>
+  <mergeCells count="10">
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="I12:M12"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="B22:F22"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="H1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="I4:M9">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B4:F9">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:F19">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:F29">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:M19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1051,7 +1720,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F19">
+  <conditionalFormatting sqref="I24:M29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
COP centré sur centre surface implant donc meilleur calcul moment
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA1B21D-6708-43C7-978C-06F7F6B57A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28913D3-11D3-404A-BE7D-9ABAF4395B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -260,14 +260,14 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -718,7 +718,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,14 +738,14 @@
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -761,13 +761,13 @@
       <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -812,19 +812,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>182.73604698252799</v>
+        <v>106.911495613464</v>
       </c>
       <c r="C4" s="9">
-        <v>169.965116238218</v>
+        <v>97.330655219946294</v>
       </c>
       <c r="D4" s="9">
-        <v>209.00959847145299</v>
+        <v>118.56451709366701</v>
       </c>
       <c r="E4" s="9">
-        <v>249.87519780755699</v>
+        <v>141.72627329487801</v>
       </c>
       <c r="F4" s="10">
-        <v>273.69375085206502</v>
+        <v>155.32248855898601</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>3</v>
@@ -850,19 +850,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="9">
-        <v>179.827394726748</v>
+        <v>104.79227649851001</v>
       </c>
       <c r="C5" s="9">
-        <v>145.31407814489799</v>
+        <v>85.476263636805797</v>
       </c>
       <c r="D5" s="9">
-        <v>190.120758225305</v>
+        <v>107.875949854089</v>
       </c>
       <c r="E5" s="9">
-        <v>250.31642299382401</v>
+        <v>142.02103745588201</v>
       </c>
       <c r="F5" s="10">
-        <v>276.630711232397</v>
+        <v>157.15788094367099</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>4</v>
@@ -888,19 +888,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="9">
-        <v>195.04023456458799</v>
+        <v>113</v>
       </c>
       <c r="C6" s="9">
-        <v>141.26001699182299</v>
+        <v>83</v>
       </c>
       <c r="D6" s="9">
-        <v>175.327907172306</v>
+        <v>100</v>
       </c>
       <c r="E6" s="9">
-        <v>255.16060531322501</v>
+        <v>145</v>
       </c>
       <c r="F6" s="10">
-        <v>283.65502062246401</v>
+        <v>161</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>5</v>
@@ -926,19 +926,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="9">
-        <v>218.01985016285201</v>
+        <v>126.16123169028999</v>
       </c>
       <c r="C7" s="9">
-        <v>144.98494010669</v>
+        <v>84.720821976112703</v>
       </c>
       <c r="D7" s="9">
-        <v>159.20782247769901</v>
+        <v>92.771827734519206</v>
       </c>
       <c r="E7" s="9">
-        <v>261.26579960812899</v>
+        <v>148.464660644887</v>
       </c>
       <c r="F7" s="10">
-        <v>292.72806844669901</v>
+        <v>166.886577087017</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>6</v>
@@ -964,19 +964,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="9">
-        <v>265.192655890808</v>
+        <v>152.80427297849999</v>
       </c>
       <c r="C8" s="9">
-        <v>171.32957880330599</v>
+        <v>99.305029193428794</v>
       </c>
       <c r="D8" s="9">
-        <v>161.342385017754</v>
+        <v>94.549009498835105</v>
       </c>
       <c r="E8" s="9">
-        <v>272.90885431698803</v>
+        <v>155.248479228273</v>
       </c>
       <c r="F8" s="10">
-        <v>368.68107850545903</v>
+        <v>254.525748019681</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>7</v>
@@ -1002,19 +1002,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="11">
-        <v>278.60638039876397</v>
+        <v>160.23988368338499</v>
       </c>
       <c r="C9" s="11">
-        <v>200.27884649179001</v>
+        <v>115.557646981895</v>
       </c>
       <c r="D9" s="11">
-        <v>192.66514587292201</v>
+        <v>112.052909095057</v>
       </c>
       <c r="E9" s="11">
-        <v>295.41908599617301</v>
+        <v>168.28102133942301</v>
       </c>
       <c r="F9" s="12">
-        <v>388.59391117002099</v>
+        <v>271.00628895696002</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>8</v>
@@ -1044,14 +1044,14 @@
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1067,13 +1067,13 @@
       <c r="H12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -1118,19 +1118,19 @@
         <v>3</v>
       </c>
       <c r="B14" s="9">
-        <v>121.059447796282</v>
+        <v>69.596156670610796</v>
       </c>
       <c r="C14" s="9">
-        <v>116.906198383478</v>
+        <v>67.163277917668694</v>
       </c>
       <c r="D14" s="9">
-        <v>137.85758780701801</v>
+        <v>79.214720520481904</v>
       </c>
       <c r="E14" s="9">
-        <v>162.691185062415</v>
+        <v>93.531162177309298</v>
       </c>
       <c r="F14" s="10">
-        <v>174.363445926016</v>
+        <v>100.295750082507</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>3</v>
@@ -1156,19 +1156,19 @@
         <v>4</v>
       </c>
       <c r="B15" s="9">
-        <v>103.94718076968</v>
+        <v>59.709474747807597</v>
       </c>
       <c r="C15" s="9">
-        <v>91.068321671400298</v>
+        <v>52.264524270759097</v>
       </c>
       <c r="D15" s="9">
-        <v>132.48928413831001</v>
+        <v>76.066620619533694</v>
       </c>
       <c r="E15" s="9">
-        <v>170.65693738371499</v>
+        <v>98.051417818185499</v>
       </c>
       <c r="F15" s="10">
-        <v>182.31319746347401</v>
+        <v>104.864665635835</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>4</v>
@@ -1194,19 +1194,19 @@
         <v>5</v>
       </c>
       <c r="B16" s="9">
-        <v>105.164634240624</v>
+        <v>60.390496379725299</v>
       </c>
       <c r="C16" s="9">
-        <v>76.0574092633031</v>
+        <v>43.637620865082802</v>
       </c>
       <c r="D16" s="9">
-        <v>126.592080341298</v>
+        <v>72.666800263838397</v>
       </c>
       <c r="E16" s="9">
-        <v>178.35476995450901</v>
+        <v>102.462185927582</v>
       </c>
       <c r="F16" s="10">
-        <v>190.69904866028401</v>
+        <v>109.74839776271899</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>5</v>
@@ -1232,19 +1232,19 @@
         <v>6</v>
       </c>
       <c r="B17" s="9">
-        <v>110.895321691419</v>
+        <v>63.668371967469199</v>
       </c>
       <c r="C17" s="9">
-        <v>64.468866028476796</v>
+        <v>36.978959204856402</v>
       </c>
       <c r="D17" s="9">
-        <v>116.521812872198</v>
+        <v>66.873879667318306</v>
       </c>
       <c r="E17" s="9">
-        <v>186.82954582293999</v>
+        <v>107.32946035523899</v>
       </c>
       <c r="F17" s="10">
-        <v>200.52271762996199</v>
+        <v>115.54566355465199</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>6</v>
@@ -1270,19 +1270,19 @@
         <v>7</v>
       </c>
       <c r="B18" s="9">
-        <v>121.063458344634</v>
+        <v>69.492181471561196</v>
       </c>
       <c r="C18" s="9">
-        <v>55.708866534578902</v>
+        <v>31.944067304912199</v>
       </c>
       <c r="D18" s="9">
-        <v>93.436026116025005</v>
+        <v>53.607611690381702</v>
       </c>
       <c r="E18" s="9">
-        <v>204.65569135918599</v>
+        <v>117.543892414147</v>
       </c>
       <c r="F18" s="10">
-        <v>236.61450822179299</v>
+        <v>149.810408619236</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>7</v>
@@ -1308,19 +1308,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="11">
-        <v>105.653555112183</v>
+        <v>60.620369451893701</v>
       </c>
       <c r="C19" s="11">
-        <v>53.066867532102101</v>
+        <v>30.411733600421101</v>
       </c>
       <c r="D19" s="11">
-        <v>97.197473959835605</v>
+        <v>55.738380821809201</v>
       </c>
       <c r="E19" s="11">
-        <v>235.43147693332199</v>
+        <v>135.14220227992899</v>
       </c>
       <c r="F19" s="12">
-        <v>289.88520078182</v>
+        <v>202.828160318622</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>8</v>
@@ -1342,44 +1342,44 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="H21" s="15" t="s">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="H21" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
       <c r="H22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
@@ -1424,19 +1424,19 @@
         <v>3</v>
       </c>
       <c r="B24" s="9">
-        <v>61.676599186245298</v>
+        <v>37.315338942853998</v>
       </c>
       <c r="C24" s="9">
-        <v>53.058917854739299</v>
+        <v>30.1673773022776</v>
       </c>
       <c r="D24" s="9">
-        <v>71.152010664434698</v>
+        <v>39.349796573185898</v>
       </c>
       <c r="E24" s="9">
-        <v>87.184012745141999</v>
+        <v>48.195111117568999</v>
       </c>
       <c r="F24" s="10">
-        <v>99.330304926048697</v>
+        <v>55.0267384764783</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>3</v>
@@ -1462,19 +1462,19 @@
         <v>4</v>
       </c>
       <c r="B25" s="9">
-        <v>75.880213957067696</v>
+        <v>45.0828017507027</v>
       </c>
       <c r="C25" s="9">
-        <v>54.245756473498602</v>
+        <v>33.211739366046601</v>
       </c>
       <c r="D25" s="9">
-        <v>57.631474086994103</v>
+        <v>31.8093292345553</v>
       </c>
       <c r="E25" s="9">
-        <v>79.659485610109101</v>
+        <v>43.969619637697399</v>
       </c>
       <c r="F25" s="10">
-        <v>94.317513768922794</v>
+        <v>52.293215307835297</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>4</v>
@@ -1500,19 +1500,19 @@
         <v>5</v>
       </c>
       <c r="B26" s="9">
-        <v>89.875600323964406</v>
+        <v>52.856528090523</v>
       </c>
       <c r="C26" s="9">
-        <v>65.202607728519993</v>
+        <v>39.254496626011097</v>
       </c>
       <c r="D26" s="9">
-        <v>48.735826831007202</v>
+        <v>27.000979138445398</v>
       </c>
       <c r="E26" s="9">
-        <v>76.805835358716095</v>
+        <v>42.393822406701297</v>
       </c>
       <c r="F26" s="10">
-        <v>92.9559719621802</v>
+        <v>51.617457767511603</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>5</v>
@@ -1538,19 +1538,19 @@
         <v>6</v>
       </c>
       <c r="B27" s="9">
-        <v>107.124528471432</v>
+        <v>62.492859722820903</v>
       </c>
       <c r="C27" s="9">
-        <v>80.516074078213506</v>
+        <v>47.741862771256301</v>
       </c>
       <c r="D27" s="9">
-        <v>42.686009605500601</v>
+        <v>25.8979480672009</v>
       </c>
       <c r="E27" s="9">
-        <v>74.436253785188597</v>
+        <v>41.135200289648097</v>
       </c>
       <c r="F27" s="10">
-        <v>92.205350816736697</v>
+        <v>51.340913532364098</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>6</v>
@@ -1576,19 +1576,19 @@
         <v>7</v>
       </c>
       <c r="B28" s="9">
-        <v>144.129197546174</v>
+        <v>83.312091506939595</v>
       </c>
       <c r="C28" s="9">
-        <v>115.620712268727</v>
+        <v>67.360961888516499</v>
       </c>
       <c r="D28" s="9">
-        <v>67.906358901729007</v>
+        <v>40.941397808453402</v>
       </c>
       <c r="E28" s="9">
-        <v>68.253162957802004</v>
+        <v>37.704586814125797</v>
       </c>
       <c r="F28" s="10">
-        <v>132.06657028366601</v>
+        <v>104.715339400445</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>7</v>
@@ -1614,19 +1614,19 @@
         <v>8</v>
       </c>
       <c r="B29" s="11">
-        <v>172.952825286581</v>
+        <v>99.619514231491294</v>
       </c>
       <c r="C29" s="11">
-        <v>147.211978959688</v>
+        <v>85.145913381474699</v>
       </c>
       <c r="D29" s="11">
-        <v>95.467671913086804</v>
+        <v>56.3145282732482</v>
       </c>
       <c r="E29" s="11">
-        <v>59.987609062850197</v>
+        <v>33.138819059493699</v>
       </c>
       <c r="F29" s="12">
-        <v>98.708710388200302</v>
+        <v>68.178128638337995</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>8</v>
@@ -1649,18 +1649,18 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="H1:M1"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="H21:M21"/>
     <mergeCell ref="I22:M22"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="H1:M1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I4:M9">
+  <conditionalFormatting sqref="B4:F9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1672,7 +1672,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F9">
+  <conditionalFormatting sqref="B14:F19">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1684,8 +1684,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F19">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="I4:M9">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:M19">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:M29">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1697,30 +1721,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:F29">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:M19">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
constant abduction speed rather than smoothed
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1B8DC5-DE25-4A28-A8F4-B77AA763C144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C834F27-8EC8-4E60-B9B8-B2F4DD8503AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="16">
   <si>
     <t>Glenoid</t>
   </si>
@@ -82,11 +82,17 @@
   <si>
     <t>Total IS shear forces on the glenoid [N]</t>
   </si>
+  <si>
+    <t>AP/IS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -222,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -260,6 +266,27 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -287,115 +314,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>539462</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>177512</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>110199</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Graphique 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{109C2552-516D-AF58-B93C-897E9D2857D3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11553826" y="0"/>
-          <a:ext cx="8782050" cy="4578290"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>690996</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>67108</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>729096</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>30739</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Graphique 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5D61D09-ED6F-C7C2-4BFD-43CF8A74131C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId4"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12467360" y="4812290"/>
-          <a:ext cx="50330100" cy="7704858"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -715,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99E3FA34-2DBA-4A8A-BF5F-CD7F590C191F}">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,47 +647,83 @@
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="H1" s="15" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="H1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-    </row>
-    <row r="2" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="P1" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="W1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+    </row>
+    <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
       <c r="H2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="P2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="21"/>
+      <c r="W2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="21"/>
+    </row>
+    <row r="3" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -806,276 +760,504 @@
       <c r="M3" s="6">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="U3" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>106.911495613464</v>
+        <v>137.156395177371</v>
       </c>
       <c r="C4" s="9">
-        <v>97.330655219946294</v>
+        <v>124.14644555753701</v>
       </c>
       <c r="D4" s="9">
-        <v>118.56451709366701</v>
+        <v>180.40066282899599</v>
       </c>
       <c r="E4" s="9">
-        <v>141.72627329487801</v>
+        <v>226.14327983329699</v>
       </c>
       <c r="F4" s="10">
-        <v>155.32248855898601</v>
+        <v>243.87161150523599</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="P4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>106.911495613464</v>
+      </c>
+      <c r="R4" s="9">
+        <v>97.330655219946294</v>
+      </c>
+      <c r="S4" s="9">
+        <v>118.56451709366701</v>
+      </c>
+      <c r="T4" s="9">
+        <v>141.72627329487801</v>
+      </c>
+      <c r="U4" s="10">
+        <v>155.32248855898601</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="9">
         <v>3094.8796477168598</v>
       </c>
-      <c r="J4" s="9">
+      <c r="Y4" s="9">
         <v>2992.8972374032401</v>
       </c>
-      <c r="K4" s="9">
+      <c r="Z4" s="9">
         <v>3695.8390605910899</v>
       </c>
-      <c r="L4" s="9">
+      <c r="AA4" s="9">
         <v>4418.3455812754501</v>
       </c>
-      <c r="M4" s="10">
+      <c r="AB4" s="10">
         <v>4834.8187391920301</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="9">
-        <v>104.79227649851001</v>
+        <v>149.67699878487699</v>
       </c>
       <c r="C5" s="9">
-        <v>85.476263636805797</v>
+        <v>114.84234244944</v>
       </c>
       <c r="D5" s="9">
-        <v>107.875949854089</v>
+        <v>177.79227946437899</v>
       </c>
       <c r="E5" s="9">
-        <v>142.02103745588201</v>
+        <v>246.045138506733</v>
       </c>
       <c r="F5" s="10">
-        <v>157.15788094367099</v>
+        <v>265.42798015076397</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="10"/>
+      <c r="P5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>104.79227649851001</v>
+      </c>
+      <c r="R5" s="9">
+        <v>85.476263636805797</v>
+      </c>
+      <c r="S5" s="9">
+        <v>107.875949854089</v>
+      </c>
+      <c r="T5" s="9">
+        <v>142.02103745588201</v>
+      </c>
+      <c r="U5" s="10">
+        <v>157.15788094367099</v>
+      </c>
+      <c r="W5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="9">
         <v>3062.6578868668398</v>
       </c>
-      <c r="J5" s="9">
+      <c r="Y5" s="9">
         <v>2442.3597758405299</v>
       </c>
-      <c r="K5" s="9">
+      <c r="Z5" s="9">
         <v>3361.3836192029999</v>
       </c>
-      <c r="L5" s="9">
+      <c r="AA5" s="9">
         <v>4424.1664384715596</v>
       </c>
-      <c r="M5" s="10">
+      <c r="AB5" s="10">
         <v>4880.5017747422498</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="9">
-        <v>113</v>
+        <v>176.09339681699899</v>
       </c>
       <c r="C6" s="9">
-        <v>83</v>
+        <v>115.30946950742801</v>
       </c>
       <c r="D6" s="9">
-        <v>100</v>
+        <v>169.340197052105</v>
       </c>
       <c r="E6" s="9">
-        <v>145</v>
+        <v>263.69577789611299</v>
       </c>
       <c r="F6" s="10">
-        <v>161</v>
+        <v>285.428814935334</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="10"/>
+      <c r="P6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>113</v>
+      </c>
+      <c r="R6" s="9">
+        <v>83</v>
+      </c>
+      <c r="S6" s="9">
+        <v>100</v>
+      </c>
+      <c r="T6" s="9">
+        <v>145</v>
+      </c>
+      <c r="U6" s="10">
+        <v>161</v>
+      </c>
+      <c r="W6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="X6" s="9">
         <v>3338.4983711975701</v>
       </c>
-      <c r="J6" s="9">
+      <c r="Y6" s="9">
         <v>2382.3632449277102</v>
       </c>
-      <c r="K6" s="9">
+      <c r="Z6" s="9">
         <v>3094.1893257229699</v>
       </c>
-      <c r="L6" s="9">
+      <c r="AA6" s="9">
         <v>4506.0088455752702</v>
       </c>
-      <c r="M6" s="10">
+      <c r="AB6" s="10">
         <v>4995.5384970136602</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="9">
-        <v>126.16123169028999</v>
+        <v>210.05125005896701</v>
       </c>
       <c r="C7" s="9">
-        <v>84.720821976112703</v>
+        <v>124.323865684278</v>
       </c>
       <c r="D7" s="9">
-        <v>92.771827734519206</v>
+        <v>161.60523301724501</v>
       </c>
       <c r="E7" s="9">
-        <v>148.464660644887</v>
+        <v>282.88400450390799</v>
       </c>
       <c r="F7" s="10">
-        <v>166.886577087017</v>
+        <v>309.14515609513899</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="10"/>
+      <c r="P7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>126.16123169028999</v>
+      </c>
+      <c r="R7" s="9">
+        <v>84.720821976112703</v>
+      </c>
+      <c r="S7" s="9">
+        <v>92.771827734519206</v>
+      </c>
+      <c r="T7" s="9">
+        <v>148.464660644887</v>
+      </c>
+      <c r="U7" s="10">
+        <v>166.886577087017</v>
+      </c>
+      <c r="W7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="9">
         <v>3749.3313662270102</v>
       </c>
-      <c r="J7" s="9">
+      <c r="Y7" s="9">
         <v>2459.75992369704</v>
       </c>
-      <c r="K7" s="9">
+      <c r="Z7" s="9">
         <v>2766.9751053119198</v>
       </c>
-      <c r="L7" s="9">
+      <c r="AA7" s="9">
         <v>4609.2774333979196</v>
       </c>
-      <c r="M7" s="10">
+      <c r="AB7" s="10">
         <v>5140.2667193444504</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="9">
-        <v>152.80427297849999</v>
+        <v>273.55208053590098</v>
       </c>
       <c r="C8" s="9">
-        <v>99.305029193428794</v>
+        <v>165.73236377836099</v>
       </c>
       <c r="D8" s="9">
-        <v>94.549009498835105</v>
+        <v>180.29276246810301</v>
       </c>
       <c r="E8" s="9">
-        <v>155.248479228273</v>
+        <v>318.79945049701098</v>
       </c>
       <c r="F8" s="10">
-        <v>254.525748019681</v>
+        <v>451.696169519823</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="10"/>
+      <c r="P8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>152.80427297849999</v>
+      </c>
+      <c r="R8" s="9">
+        <v>99.305029193428794</v>
+      </c>
+      <c r="S8" s="9">
+        <v>94.549009498835105</v>
+      </c>
+      <c r="T8" s="9">
+        <v>155.248479228273</v>
+      </c>
+      <c r="U8" s="10">
+        <v>254.525748019681</v>
+      </c>
+      <c r="W8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X8" s="9">
         <v>4587.2809351962296</v>
       </c>
-      <c r="J8" s="9">
+      <c r="Y8" s="9">
         <v>2939.7775350970301</v>
       </c>
-      <c r="K8" s="9">
+      <c r="Z8" s="9">
         <v>2726.2602252619899</v>
       </c>
-      <c r="L8" s="9">
+      <c r="AA8" s="9">
         <v>4806.6538656575703</v>
       </c>
-      <c r="M8" s="10">
+      <c r="AB8" s="10">
         <v>5075.2425786429103</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="11">
-        <v>160.23988368338499</v>
+        <v>288.948484310982</v>
       </c>
       <c r="C9" s="11">
-        <v>115.557646981895</v>
+        <v>203.874519329148</v>
       </c>
       <c r="D9" s="11">
-        <v>112.052909095057</v>
+        <v>223.56785961402301</v>
       </c>
       <c r="E9" s="11">
-        <v>168.28102133942301</v>
+        <v>354.29472803019701</v>
       </c>
       <c r="F9" s="12">
-        <v>271.00628895696002</v>
+        <v>591.82297679834801</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="12"/>
+      <c r="P9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>160.23988368338499</v>
+      </c>
+      <c r="R9" s="11">
+        <v>115.557646981895</v>
+      </c>
+      <c r="S9" s="11">
+        <v>112.052909095057</v>
+      </c>
+      <c r="T9" s="11">
+        <v>168.28102133942301</v>
+      </c>
+      <c r="U9" s="12">
+        <v>271.00628895696002</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="11">
         <v>4831.28558021957</v>
       </c>
-      <c r="J9" s="11">
+      <c r="Y9" s="11">
         <v>3458.00814326102</v>
       </c>
-      <c r="K9" s="11">
+      <c r="Z9" s="11">
         <v>3290.29537868836</v>
       </c>
-      <c r="L9" s="11">
+      <c r="AA9" s="11">
         <v>5192.5688422368403</v>
       </c>
-      <c r="M9" s="12">
+      <c r="AB9" s="12">
         <v>5517.9643903629003</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="H11" s="15" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="H11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="P11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="W11" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="22"/>
+    </row>
+    <row r="12" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="4"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
       <c r="H12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="P12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="4"/>
+      <c r="W12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="20"/>
+      <c r="Z12" s="20"/>
+      <c r="AA12" s="20"/>
+      <c r="AB12" s="21"/>
+    </row>
+    <row r="13" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
@@ -1112,276 +1294,444 @@
       <c r="M13" s="6">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="U13" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="AB13" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="9">
-        <v>69.596156670610796</v>
-      </c>
-      <c r="C14" s="9">
-        <v>67.163277917668694</v>
-      </c>
-      <c r="D14" s="9">
-        <v>79.214720520481904</v>
-      </c>
-      <c r="E14" s="9">
-        <v>93.531162177309298</v>
-      </c>
-      <c r="F14" s="10">
-        <v>100.295750082507</v>
-      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
       <c r="H14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="9">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="10"/>
+      <c r="P14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>69.596156670610796</v>
+      </c>
+      <c r="R14" s="9">
+        <v>67.163277917668694</v>
+      </c>
+      <c r="S14" s="9">
+        <v>79.214720520481904</v>
+      </c>
+      <c r="T14" s="9">
+        <v>93.531162177309298</v>
+      </c>
+      <c r="U14" s="10">
+        <v>100.295750082507</v>
+      </c>
+      <c r="W14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X14" s="9">
         <v>994.33715279148305</v>
       </c>
-      <c r="J14" s="9">
+      <c r="Y14" s="9">
         <v>962.57395308446496</v>
       </c>
-      <c r="K14" s="9">
+      <c r="Z14" s="9">
         <v>1302.2236597147</v>
       </c>
-      <c r="L14" s="9">
+      <c r="AA14" s="9">
         <v>1595.48750433234</v>
       </c>
-      <c r="M14" s="10">
+      <c r="AB14" s="10">
         <v>1811.6474802733101</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="9">
-        <v>59.709474747807597</v>
-      </c>
-      <c r="C15" s="9">
-        <v>52.264524270759097</v>
-      </c>
-      <c r="D15" s="9">
-        <v>76.066620619533694</v>
-      </c>
-      <c r="E15" s="9">
-        <v>98.051417818185499</v>
-      </c>
-      <c r="F15" s="10">
-        <v>104.864665635835</v>
-      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
       <c r="H15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="10"/>
+      <c r="P15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>59.709474747807597</v>
+      </c>
+      <c r="R15" s="9">
+        <v>52.264524270759097</v>
+      </c>
+      <c r="S15" s="9">
+        <v>76.066620619533694</v>
+      </c>
+      <c r="T15" s="9">
+        <v>98.051417818185499</v>
+      </c>
+      <c r="U15" s="10">
+        <v>104.864665635835</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15" s="9">
         <v>1257.03723291285</v>
       </c>
-      <c r="J15" s="9">
+      <c r="Y15" s="9">
         <v>858.531310508243</v>
       </c>
-      <c r="K15" s="9">
+      <c r="Z15" s="9">
         <v>1058.4177612937301</v>
       </c>
-      <c r="L15" s="9">
+      <c r="AA15" s="9">
         <v>1460.6758439601399</v>
       </c>
-      <c r="M15" s="10">
+      <c r="AB15" s="10">
         <v>1719.33721034884</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="9">
-        <v>60.390496379725299</v>
-      </c>
-      <c r="C16" s="9">
-        <v>43.637620865082802</v>
-      </c>
-      <c r="D16" s="9">
-        <v>72.666800263838397</v>
-      </c>
-      <c r="E16" s="9">
-        <v>102.462185927582</v>
-      </c>
-      <c r="F16" s="10">
-        <v>109.74839776271899</v>
-      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
       <c r="H16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="10"/>
+      <c r="P16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>60.390496379725299</v>
+      </c>
+      <c r="R16" s="9">
+        <v>43.637620865082802</v>
+      </c>
+      <c r="S16" s="9">
+        <v>72.666800263838397</v>
+      </c>
+      <c r="T16" s="9">
+        <v>102.462185927582</v>
+      </c>
+      <c r="U16" s="10">
+        <v>109.74839776271899</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="X16" s="9">
         <v>1510.9825401404601</v>
       </c>
-      <c r="J16" s="9">
+      <c r="Y16" s="9">
         <v>1059.1065756126</v>
       </c>
-      <c r="K16" s="9">
+      <c r="Z16" s="9">
         <v>893.15748582663798</v>
       </c>
-      <c r="L16" s="9">
+      <c r="AA16" s="9">
         <v>1408.3523546802801</v>
       </c>
-      <c r="M16" s="10">
+      <c r="AB16" s="10">
         <v>1691.4302971130601</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="9">
-        <v>63.668371967469199</v>
-      </c>
-      <c r="C17" s="9">
-        <v>36.978959204856402</v>
-      </c>
-      <c r="D17" s="9">
-        <v>66.873879667318306</v>
-      </c>
-      <c r="E17" s="9">
-        <v>107.32946035523899</v>
-      </c>
-      <c r="F17" s="10">
-        <v>115.54566355465199</v>
-      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
       <c r="H17" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="10"/>
+      <c r="P17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>63.668371967469199</v>
+      </c>
+      <c r="R17" s="9">
+        <v>36.978959204856402</v>
+      </c>
+      <c r="S17" s="9">
+        <v>66.873879667318306</v>
+      </c>
+      <c r="T17" s="9">
+        <v>107.32946035523899</v>
+      </c>
+      <c r="U17" s="10">
+        <v>115.54566355465199</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X17" s="9">
         <v>1821.7007652494599</v>
       </c>
-      <c r="J17" s="9">
+      <c r="Y17" s="9">
         <v>1337.72291048804</v>
       </c>
-      <c r="K17" s="9">
+      <c r="Z17" s="9">
         <v>740.528852051493</v>
       </c>
-      <c r="L17" s="9">
+      <c r="AA17" s="9">
         <v>1364.3759857366499</v>
       </c>
-      <c r="M17" s="10">
+      <c r="AB17" s="10">
         <v>1671.8155325970999</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="9">
-        <v>69.492181471561196</v>
-      </c>
-      <c r="C18" s="9">
-        <v>31.944067304912199</v>
-      </c>
-      <c r="D18" s="9">
-        <v>53.607611690381702</v>
-      </c>
-      <c r="E18" s="9">
-        <v>117.543892414147</v>
-      </c>
-      <c r="F18" s="10">
-        <v>149.810408619236</v>
-      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
       <c r="H18" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
+      <c r="P18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>69.492181471561196</v>
+      </c>
+      <c r="R18" s="9">
+        <v>31.944067304912199</v>
+      </c>
+      <c r="S18" s="9">
+        <v>53.607611690381702</v>
+      </c>
+      <c r="T18" s="9">
+        <v>117.543892414147</v>
+      </c>
+      <c r="U18" s="10">
+        <v>149.810408619236</v>
+      </c>
+      <c r="W18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X18" s="9">
         <v>2482.3308587442798</v>
       </c>
-      <c r="J18" s="9">
+      <c r="Y18" s="9">
         <v>1969.7857298045101</v>
       </c>
-      <c r="K18" s="9">
+      <c r="Z18" s="9">
         <v>1100.6106568683899</v>
       </c>
-      <c r="L18" s="9">
+      <c r="AA18" s="9">
         <v>1251.0702352478199</v>
       </c>
-      <c r="M18" s="10">
+      <c r="AB18" s="10">
         <v>1163.1522427815</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="11">
-        <v>60.620369451893701</v>
-      </c>
-      <c r="C19" s="11">
-        <v>30.411733600421101</v>
-      </c>
-      <c r="D19" s="11">
-        <v>55.738380821809201</v>
-      </c>
-      <c r="E19" s="11">
-        <v>135.14220227992899</v>
-      </c>
-      <c r="F19" s="12">
-        <v>202.828160318622</v>
-      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
       <c r="H19" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12"/>
+      <c r="P19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>60.620369451893701</v>
+      </c>
+      <c r="R19" s="11">
+        <v>30.411733600421101</v>
+      </c>
+      <c r="S19" s="11">
+        <v>55.738380821809201</v>
+      </c>
+      <c r="T19" s="11">
+        <v>135.14220227992899</v>
+      </c>
+      <c r="U19" s="12">
+        <v>202.828160318622</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X19" s="11">
         <v>2993.1963695955101</v>
       </c>
-      <c r="J19" s="11">
+      <c r="Y19" s="11">
         <v>2533.30879911078</v>
       </c>
-      <c r="K19" s="11">
+      <c r="Z19" s="11">
         <v>1598.0874955036099</v>
       </c>
-      <c r="L19" s="11">
+      <c r="AA19" s="11">
         <v>1099.1290604656799</v>
       </c>
-      <c r="M19" s="12">
+      <c r="AB19" s="12">
         <v>1737.07657197458</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="H21" s="15" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="H21" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="P21" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="22"/>
+      <c r="T21" s="22"/>
+      <c r="U21" s="22"/>
+      <c r="W21" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="22"/>
+      <c r="AA21" s="22"/>
+      <c r="AB21" s="22"/>
+    </row>
+    <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="14"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="H22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I22" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="P22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="21"/>
+      <c r="W22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="21"/>
+    </row>
+    <row r="23" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>1</v>
       </c>
@@ -1418,249 +1768,1080 @@
       <c r="M23" s="6">
         <v>16.95</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="P23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0</v>
+      </c>
+      <c r="T23" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="U23" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="Y23" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="Z23" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="AB23" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="9">
-        <v>37.315338942853998</v>
-      </c>
-      <c r="C24" s="9">
-        <v>30.1673773022776</v>
-      </c>
-      <c r="D24" s="9">
-        <v>39.349796573185898</v>
-      </c>
-      <c r="E24" s="9">
-        <v>48.195111117568999</v>
-      </c>
-      <c r="F24" s="10">
-        <v>55.0267384764783</v>
-      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
       <c r="H24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="10"/>
+      <c r="P24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="9">
+        <v>37.315338942853998</v>
+      </c>
+      <c r="R24" s="9">
+        <v>30.1673773022776</v>
+      </c>
+      <c r="S24" s="9">
+        <v>39.349796573185898</v>
+      </c>
+      <c r="T24" s="9">
+        <v>48.195111117568999</v>
+      </c>
+      <c r="U24" s="10">
+        <v>55.0267384764783</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X24" s="9">
         <v>2100.5424949253802</v>
       </c>
-      <c r="J24" s="9">
+      <c r="Y24" s="9">
         <v>2030.32328431878</v>
       </c>
-      <c r="K24" s="9">
+      <c r="Z24" s="9">
         <v>2393.6154008763901</v>
       </c>
-      <c r="L24" s="9">
+      <c r="AA24" s="9">
         <v>2822.8580769431101</v>
       </c>
-      <c r="M24" s="10">
+      <c r="AB24" s="10">
         <v>3023.17125891871</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="9">
-        <v>45.0828017507027</v>
-      </c>
-      <c r="C25" s="9">
-        <v>33.211739366046601</v>
-      </c>
-      <c r="D25" s="9">
-        <v>31.8093292345553</v>
-      </c>
-      <c r="E25" s="9">
-        <v>43.969619637697399</v>
-      </c>
-      <c r="F25" s="10">
-        <v>52.293215307835297</v>
-      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
       <c r="H25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="10"/>
+      <c r="P25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="9">
+        <v>45.0828017507027</v>
+      </c>
+      <c r="R25" s="9">
+        <v>33.211739366046601</v>
+      </c>
+      <c r="S25" s="9">
+        <v>31.8093292345553</v>
+      </c>
+      <c r="T25" s="9">
+        <v>43.969619637697399</v>
+      </c>
+      <c r="U25" s="10">
+        <v>52.293215307835297</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X25" s="9">
         <v>1805.6206539539901</v>
       </c>
-      <c r="J25" s="9">
+      <c r="Y25" s="9">
         <v>1583.8284653322901</v>
       </c>
-      <c r="K25" s="9">
+      <c r="Z25" s="9">
         <v>2302.9658579092702</v>
       </c>
-      <c r="L25" s="9">
+      <c r="AA25" s="9">
         <v>2963.4905945114201</v>
       </c>
-      <c r="M25" s="10">
+      <c r="AB25" s="10">
         <v>3161.1645643934098</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="9">
-        <v>52.856528090523</v>
-      </c>
-      <c r="C26" s="9">
-        <v>39.254496626011097</v>
-      </c>
-      <c r="D26" s="9">
-        <v>27.000979138445398</v>
-      </c>
-      <c r="E26" s="9">
-        <v>42.393822406701297</v>
-      </c>
-      <c r="F26" s="10">
-        <v>51.617457767511603</v>
-      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10"/>
       <c r="H26" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="10"/>
+      <c r="P26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="9">
+        <v>52.856528090523</v>
+      </c>
+      <c r="R26" s="9">
+        <v>39.254496626011097</v>
+      </c>
+      <c r="S26" s="9">
+        <v>27.000979138445398</v>
+      </c>
+      <c r="T26" s="9">
+        <v>42.393822406701297</v>
+      </c>
+      <c r="U26" s="10">
+        <v>51.617457767511603</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="X26" s="9">
         <v>1827.5158310571001</v>
       </c>
-      <c r="J26" s="9">
+      <c r="Y26" s="9">
         <v>1323.25666931511</v>
       </c>
-      <c r="K26" s="9">
+      <c r="Z26" s="9">
         <v>2201.03183989633</v>
       </c>
-      <c r="L26" s="9">
+      <c r="AA26" s="9">
         <v>3097.6564908949799</v>
       </c>
-      <c r="M26" s="10">
+      <c r="AB26" s="10">
         <v>3304.1081999006001</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="9">
-        <v>62.492859722820903</v>
-      </c>
-      <c r="C27" s="9">
-        <v>47.741862771256301</v>
-      </c>
-      <c r="D27" s="9">
-        <v>25.8979480672009</v>
-      </c>
-      <c r="E27" s="9">
-        <v>41.135200289648097</v>
-      </c>
-      <c r="F27" s="10">
-        <v>51.340913532364098</v>
-      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
       <c r="H27" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="10"/>
+      <c r="P27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="9">
+        <v>62.492859722820903</v>
+      </c>
+      <c r="R27" s="9">
+        <v>47.741862771256301</v>
+      </c>
+      <c r="S27" s="9">
+        <v>25.8979480672009</v>
+      </c>
+      <c r="T27" s="9">
+        <v>41.135200289648097</v>
+      </c>
+      <c r="U27" s="10">
+        <v>51.340913532364098</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X27" s="9">
         <v>1927.6306009775501</v>
       </c>
-      <c r="J27" s="9">
+      <c r="Y27" s="9">
         <v>1122.0370132089899</v>
       </c>
-      <c r="K27" s="9">
+      <c r="Z27" s="9">
         <v>2026.44625326043</v>
       </c>
-      <c r="L27" s="9">
+      <c r="AA27" s="9">
         <v>3244.9014476612601</v>
       </c>
-      <c r="M27" s="10">
+      <c r="AB27" s="10">
         <v>3468.4511867473402</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="9">
-        <v>83.312091506939595</v>
-      </c>
-      <c r="C28" s="9">
-        <v>67.360961888516499</v>
-      </c>
-      <c r="D28" s="9">
-        <v>40.941397808453402</v>
-      </c>
-      <c r="E28" s="9">
-        <v>37.704586814125797</v>
-      </c>
-      <c r="F28" s="10">
-        <v>104.715339400445</v>
-      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
       <c r="H28" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="10"/>
+      <c r="P28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="9">
+        <v>83.312091506939595</v>
+      </c>
+      <c r="R28" s="9">
+        <v>67.360961888516499</v>
+      </c>
+      <c r="S28" s="9">
+        <v>40.941397808453402</v>
+      </c>
+      <c r="T28" s="9">
+        <v>37.704586814125797</v>
+      </c>
+      <c r="U28" s="10">
+        <v>104.715339400445</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X28" s="9">
         <v>2104.9500764519498</v>
       </c>
-      <c r="J28" s="9">
+      <c r="Y28" s="9">
         <v>969.99180529251896</v>
       </c>
-      <c r="K28" s="9">
+      <c r="Z28" s="9">
         <v>1625.6495683936</v>
       </c>
-      <c r="L28" s="9">
+      <c r="AA28" s="9">
         <v>3555.5836304097502</v>
       </c>
-      <c r="M28" s="10">
+      <c r="AB28" s="10">
         <v>3912.0903358614</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="11">
-        <v>99.619514231491294</v>
-      </c>
-      <c r="C29" s="11">
-        <v>85.145913381474699</v>
-      </c>
-      <c r="D29" s="11">
-        <v>56.3145282732482</v>
-      </c>
-      <c r="E29" s="11">
-        <v>33.138819059493699</v>
-      </c>
-      <c r="F29" s="12">
-        <v>68.178128638337995</v>
-      </c>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="12"/>
       <c r="H29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="12"/>
+      <c r="P29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="11">
+        <v>99.619514231491294</v>
+      </c>
+      <c r="R29" s="11">
+        <v>85.145913381474699</v>
+      </c>
+      <c r="S29" s="11">
+        <v>56.3145282732482</v>
+      </c>
+      <c r="T29" s="11">
+        <v>33.138819059493699</v>
+      </c>
+      <c r="U29" s="12">
+        <v>68.178128638337995</v>
+      </c>
+      <c r="W29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X29" s="11">
         <v>1838.0892106240599</v>
       </c>
-      <c r="J29" s="11">
+      <c r="Y29" s="11">
         <v>924.69934415024397</v>
       </c>
-      <c r="K29" s="11">
+      <c r="Z29" s="11">
         <v>1692.20788318474</v>
       </c>
-      <c r="L29" s="11">
+      <c r="AA29" s="11">
         <v>4093.4397817711501</v>
       </c>
-      <c r="M29" s="12">
+      <c r="AB29" s="12">
         <v>3780.8878183883198</v>
       </c>
     </row>
+    <row r="31" spans="1:28" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="H31" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="22"/>
+      <c r="P31" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="22"/>
+      <c r="R31" s="22"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="22"/>
+      <c r="U31" s="22"/>
+      <c r="W31" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="X31" s="22"/>
+      <c r="Y31" s="22"/>
+      <c r="Z31" s="22"/>
+      <c r="AA31" s="22"/>
+      <c r="AB31" s="22"/>
+    </row>
+    <row r="32" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
+      <c r="H32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="21"/>
+      <c r="P32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="21"/>
+      <c r="W32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="X32" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y32" s="20"/>
+      <c r="Z32" s="20"/>
+      <c r="AA32" s="20"/>
+      <c r="AB32" s="21"/>
+    </row>
+    <row r="33" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="F33" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="M33" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="P33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="R33" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="U33" s="6">
+        <v>16.95</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X33" s="1">
+        <v>-12.1</v>
+      </c>
+      <c r="Y33" s="1">
+        <v>-6.6</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>7.85</v>
+      </c>
+      <c r="AB33" s="6">
+        <v>16.95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="14"/>
+      <c r="H34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="14"/>
+      <c r="P34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="13">
+        <f>Q14/Q24</f>
+        <v>1.8650817235559018</v>
+      </c>
+      <c r="R34" s="13">
+        <f t="shared" ref="R34:U34" si="0">R14/R24</f>
+        <v>2.2263545566023715</v>
+      </c>
+      <c r="S34" s="13">
+        <f t="shared" si="0"/>
+        <v>2.0130909793434899</v>
+      </c>
+      <c r="T34" s="13">
+        <f t="shared" si="0"/>
+        <v>1.9406773842505685</v>
+      </c>
+      <c r="U34" s="14">
+        <f t="shared" si="0"/>
+        <v>1.8226729924285694</v>
+      </c>
+      <c r="W34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="X34" s="13">
+        <f>X14/X24</f>
+        <v>0.47337159576331539</v>
+      </c>
+      <c r="Y34" s="13">
+        <f t="shared" ref="Y34:AB34" si="1">Y14/Y24</f>
+        <v>0.47409885928950996</v>
+      </c>
+      <c r="Z34" s="13">
+        <f t="shared" si="1"/>
+        <v>0.54404047502280795</v>
+      </c>
+      <c r="AA34" s="13">
+        <f t="shared" si="1"/>
+        <v>0.56520287624948651</v>
+      </c>
+      <c r="AB34" s="14">
+        <f t="shared" si="1"/>
+        <v>0.59925400353312352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="16"/>
+      <c r="H35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
+      <c r="P35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q35" s="15">
+        <f t="shared" ref="Q35:U35" si="2">Q15/Q25</f>
+        <v>1.3244401951322138</v>
+      </c>
+      <c r="R35" s="15">
+        <f t="shared" si="2"/>
+        <v>1.5736762141458558</v>
+      </c>
+      <c r="S35" s="15">
+        <f t="shared" si="2"/>
+        <v>2.3913305451565621</v>
+      </c>
+      <c r="T35" s="15">
+        <f t="shared" si="2"/>
+        <v>2.2299810329521481</v>
+      </c>
+      <c r="U35" s="16">
+        <f t="shared" si="2"/>
+        <v>2.0053206714967997</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X35" s="15">
+        <f t="shared" ref="X35:AB35" si="3">X15/X25</f>
+        <v>0.69618013626514552</v>
+      </c>
+      <c r="Y35" s="15">
+        <f t="shared" si="3"/>
+        <v>0.5420607908622993</v>
+      </c>
+      <c r="Z35" s="15">
+        <f t="shared" si="3"/>
+        <v>0.45958899375720946</v>
+      </c>
+      <c r="AA35" s="15">
+        <f t="shared" si="3"/>
+        <v>0.49289032557262297</v>
+      </c>
+      <c r="AB35" s="16">
+        <f t="shared" si="3"/>
+        <v>0.54389361114414503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="16"/>
+      <c r="H36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="16"/>
+      <c r="P36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="15">
+        <f t="shared" ref="Q36:U36" si="4">Q16/Q26</f>
+        <v>1.1425361929996518</v>
+      </c>
+      <c r="R36" s="15">
+        <f t="shared" si="4"/>
+        <v>1.1116591630464909</v>
+      </c>
+      <c r="S36" s="15">
+        <f t="shared" si="4"/>
+        <v>2.6912653756460121</v>
+      </c>
+      <c r="T36" s="15">
+        <f t="shared" si="4"/>
+        <v>2.4169131281586336</v>
+      </c>
+      <c r="U36" s="16">
+        <f t="shared" si="4"/>
+        <v>2.1261875828335626</v>
+      </c>
+      <c r="W36" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="X36" s="15">
+        <f t="shared" ref="X36:AB36" si="5">X16/X26</f>
+        <v>0.82679586926831383</v>
+      </c>
+      <c r="Y36" s="15">
+        <f t="shared" si="5"/>
+        <v>0.80037879284656954</v>
+      </c>
+      <c r="Z36" s="15">
+        <f t="shared" si="5"/>
+        <v>0.40579035234161187</v>
+      </c>
+      <c r="AA36" s="15">
+        <f t="shared" si="5"/>
+        <v>0.45465091394732948</v>
+      </c>
+      <c r="AB36" s="16">
+        <f t="shared" si="5"/>
+        <v>0.51191734494770624</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="16"/>
+      <c r="H37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="16"/>
+      <c r="P37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q37" s="15">
+        <f t="shared" ref="Q37:U37" si="6">Q17/Q27</f>
+        <v>1.0188103448915944</v>
+      </c>
+      <c r="R37" s="15">
+        <f t="shared" si="6"/>
+        <v>0.77456046032456305</v>
+      </c>
+      <c r="S37" s="15">
+        <f t="shared" si="6"/>
+        <v>2.5822076518877721</v>
+      </c>
+      <c r="T37" s="15">
+        <f t="shared" si="6"/>
+        <v>2.6091877418729634</v>
+      </c>
+      <c r="U37" s="16">
+        <f t="shared" si="6"/>
+        <v>2.2505572185001097</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X37" s="15">
+        <f t="shared" ref="X37:AB37" si="7">X17/X27</f>
+        <v>0.94504661024037984</v>
+      </c>
+      <c r="Y37" s="15">
+        <f t="shared" si="7"/>
+        <v>1.1922270787326306</v>
+      </c>
+      <c r="Z37" s="15">
+        <f t="shared" si="7"/>
+        <v>0.36543226885984598</v>
+      </c>
+      <c r="AA37" s="15">
+        <f t="shared" si="7"/>
+        <v>0.42046761904587715</v>
+      </c>
+      <c r="AB37" s="16">
+        <f t="shared" si="7"/>
+        <v>0.48200636035616307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="16"/>
+      <c r="H38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="16"/>
+      <c r="P38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q38" s="15">
+        <f t="shared" ref="Q38:U38" si="8">Q18/Q28</f>
+        <v>0.83411879613864637</v>
+      </c>
+      <c r="R38" s="15">
+        <f t="shared" si="8"/>
+        <v>0.47422225587841449</v>
+      </c>
+      <c r="S38" s="15">
+        <f t="shared" si="8"/>
+        <v>1.3093742412310367</v>
+      </c>
+      <c r="T38" s="15">
+        <f t="shared" si="8"/>
+        <v>3.1174958366102525</v>
+      </c>
+      <c r="U38" s="16">
+        <f t="shared" si="8"/>
+        <v>1.4306443495001397</v>
+      </c>
+      <c r="W38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="X38" s="15">
+        <f t="shared" ref="X38:AB38" si="9">X18/X28</f>
+        <v>1.1792825333551062</v>
+      </c>
+      <c r="Y38" s="15">
+        <f t="shared" si="9"/>
+        <v>2.0307240938086943</v>
+      </c>
+      <c r="Z38" s="15">
+        <f t="shared" si="9"/>
+        <v>0.67702823429281134</v>
+      </c>
+      <c r="AA38" s="15">
+        <f t="shared" si="9"/>
+        <v>0.35186072535260404</v>
+      </c>
+      <c r="AB38" s="16">
+        <f t="shared" si="9"/>
+        <v>0.29732243964795524</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="18"/>
+      <c r="H39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="18"/>
+      <c r="P39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q39" s="17">
+        <f t="shared" ref="Q39:U39" si="10">Q19/Q29</f>
+        <v>0.60851902279935677</v>
+      </c>
+      <c r="R39" s="17">
+        <f t="shared" si="10"/>
+        <v>0.35717196977110377</v>
+      </c>
+      <c r="S39" s="17">
+        <f t="shared" si="10"/>
+        <v>0.98976911519806354</v>
+      </c>
+      <c r="T39" s="17">
+        <f t="shared" si="10"/>
+        <v>4.0780633141244387</v>
+      </c>
+      <c r="U39" s="18">
+        <f t="shared" si="10"/>
+        <v>2.9749740036802281</v>
+      </c>
+      <c r="W39" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="X39" s="17">
+        <f t="shared" ref="X39:AB39" si="11">X19/X29</f>
+        <v>1.6284282353081618</v>
+      </c>
+      <c r="Y39" s="17">
+        <f t="shared" si="11"/>
+        <v>2.7396026774938118</v>
+      </c>
+      <c r="Z39" s="17">
+        <f t="shared" si="11"/>
+        <v>0.94438012692388884</v>
+      </c>
+      <c r="AA39" s="17">
+        <f t="shared" si="11"/>
+        <v>0.26850988876404297</v>
+      </c>
+      <c r="AB39" s="18">
+        <f t="shared" si="11"/>
+        <v>0.45943615769987173</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="31">
+    <mergeCell ref="P31:U31"/>
+    <mergeCell ref="W31:AB31"/>
+    <mergeCell ref="Q32:U32"/>
+    <mergeCell ref="X32:AB32"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="X12:AB12"/>
+    <mergeCell ref="P21:U21"/>
+    <mergeCell ref="W21:AB21"/>
+    <mergeCell ref="Q22:U22"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="X2:AB2"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="W11:AB11"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="I2:M2"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="H11:M11"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="I32:M32"/>
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="H21:M21"/>
     <mergeCell ref="I22:M22"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="B22:F22"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:F9">
+  <conditionalFormatting sqref="B14:F19">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24:F29">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:F39">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:M9">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:M19">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I24:M29">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34:M39">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:U9">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14:U19">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q24:U29">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q34:U39">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:AB9">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X14:AB19">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1672,7 +2853,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F19">
+  <conditionalFormatting sqref="X24:AB29">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1684,7 +2865,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B24:F29">
+  <conditionalFormatting sqref="X34:AB39">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:F9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1696,43 +2889,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:M9">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:M19">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I24:M29">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout save to excel
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C834F27-8EC8-4E60-B9B8-B2F4DD8503AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A942B22-194B-4AA0-9AA0-A706552D587C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
   <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,11 +819,21 @@
       <c r="H4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
+      <c r="I4" s="9">
+        <v>3852.6358305144399</v>
+      </c>
+      <c r="J4" s="9">
+        <v>3886.8614198381401</v>
+      </c>
+      <c r="K4" s="9">
+        <v>5711.1949775252497</v>
+      </c>
+      <c r="L4" s="9">
+        <v>7132.6198831584798</v>
+      </c>
+      <c r="M4" s="10">
+        <v>7670.3851424714703</v>
+      </c>
       <c r="P4" s="7" t="s">
         <v>3</v>
       </c>
@@ -883,11 +893,21 @@
       <c r="H5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="10"/>
+      <c r="I5" s="9">
+        <v>4302.4431323520403</v>
+      </c>
+      <c r="J5" s="9">
+        <v>3168.0107132970802</v>
+      </c>
+      <c r="K5" s="9">
+        <v>5613.5523332412704</v>
+      </c>
+      <c r="L5" s="9">
+        <v>7733.9349808274601</v>
+      </c>
+      <c r="M5" s="10">
+        <v>8308.1378704456602</v>
+      </c>
       <c r="P5" s="7" t="s">
         <v>4</v>
       </c>
@@ -947,11 +967,21 @@
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
+      <c r="I6" s="9">
+        <v>5149.4458870725002</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3226.2202383661602</v>
+      </c>
+      <c r="K6" s="9">
+        <v>5323.1651638346402</v>
+      </c>
+      <c r="L6" s="9">
+        <v>8262.5852476171094</v>
+      </c>
+      <c r="M6" s="10">
+        <v>8889.24394139182</v>
+      </c>
       <c r="P6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1011,11 +1041,21 @@
       <c r="H7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="10"/>
+      <c r="I7" s="9">
+        <v>6223.6801328150696</v>
+      </c>
+      <c r="J7" s="9">
+        <v>3551.4517577358401</v>
+      </c>
+      <c r="K7" s="9">
+        <v>4869.8091767357</v>
+      </c>
+      <c r="L7" s="9">
+        <v>8840.2381634644407</v>
+      </c>
+      <c r="M7" s="10">
+        <v>9564.2249611155694</v>
+      </c>
       <c r="P7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1075,11 +1115,21 @@
       <c r="H8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="10"/>
+      <c r="I8" s="9">
+        <v>8216.3184893125908</v>
+      </c>
+      <c r="J8" s="9">
+        <v>4896.2539788139602</v>
+      </c>
+      <c r="K8" s="9">
+        <v>5180.4819909731204</v>
+      </c>
+      <c r="L8" s="9">
+        <v>9922.4508294343195</v>
+      </c>
+      <c r="M8" s="10">
+        <v>10140.121829494499</v>
+      </c>
       <c r="P8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1139,11 +1189,21 @@
       <c r="H9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="12"/>
+      <c r="I9" s="11">
+        <v>8712.2991309537902</v>
+      </c>
+      <c r="J9" s="11">
+        <v>6101.0087343801097</v>
+      </c>
+      <c r="K9" s="11">
+        <v>6567.5330099508801</v>
+      </c>
+      <c r="L9" s="11">
+        <v>10983.1622659615</v>
+      </c>
+      <c r="M9" s="12">
+        <v>10980.1522210362</v>
+      </c>
       <c r="P9" s="8" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Meilleur utilisation 3d slicer et template position glène
</commit_message>
<xml_diff>
--- a/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
+++ b/Application/Validation/EpauleFDK/Output/Resultats FDK/Scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Documents\Gitkraken\EpauleFDK\Application\Validation\EpauleFDK\Output\Resultats FDK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FC4875-9F4B-4F5A-9EAD-2B0CD2D82553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CADE3C-66FB-4B73-8D12-218651B19255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE57FB80-DC25-4055-B570-F4781C35C020}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -658,73 +658,73 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:AI67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,35 +1081,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="37"/>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
@@ -1123,34 +1123,34 @@
     </row>
     <row r="2" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="33"/>
       <c r="I2" s="13"/>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="40"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="59"/>
       <c r="O2" s="33"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
       <c r="S2" s="13"/>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="40"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="59"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
@@ -1774,33 +1774,33 @@
       <c r="AI12" s="5"/>
     </row>
     <row r="13" spans="1:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="I13" s="41" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="I13" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="5"/>
-      <c r="S13" s="38" t="s">
+      <c r="S13" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="T13" s="38"/>
-      <c r="U13" s="38"/>
-      <c r="V13" s="38"/>
-      <c r="W13" s="38"/>
-      <c r="X13" s="38"/>
-      <c r="Y13" s="38"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="58"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="58"/>
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
@@ -1814,32 +1814,32 @@
     </row>
     <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="59"/>
       <c r="I14" s="13"/>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="40"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="59"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="5"/>
       <c r="S14" s="13"/>
-      <c r="T14" s="39" t="s">
+      <c r="T14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
-      <c r="W14" s="39"/>
-      <c r="X14" s="39"/>
-      <c r="Y14" s="40"/>
+      <c r="U14" s="54"/>
+      <c r="V14" s="54"/>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="59"/>
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
@@ -2393,22 +2393,22 @@
       <c r="AI22" s="5"/>
     </row>
     <row r="23" spans="1:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="I23" s="38" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="I23" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="38"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
@@ -2431,33 +2431,33 @@
     </row>
     <row r="24" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="59"/>
       <c r="I24" s="13"/>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="40"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="59"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="5"/>
       <c r="S24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="T24" s="39" t="s">
+      <c r="T24" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="U24" s="39"/>
-      <c r="V24" s="39"/>
-      <c r="W24" s="39"/>
-      <c r="X24" s="39"/>
+      <c r="U24" s="54"/>
+      <c r="V24" s="54"/>
+      <c r="W24" s="54"/>
+      <c r="X24" s="54"/>
       <c r="Y24" s="5"/>
       <c r="Z24" s="5"/>
       <c r="AA24" s="5"/>
@@ -2581,19 +2581,19 @@
       <c r="S26" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="T26" s="42" t="s">
+      <c r="T26" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="U26" s="42" t="s">
+      <c r="U26" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="V26" s="42" t="s">
+      <c r="V26" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="W26" s="42" t="s">
+      <c r="W26" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="X26" s="42" t="s">
+      <c r="X26" s="38" t="s">
         <v>35</v>
       </c>
       <c r="Y26" s="5"/>
@@ -2650,19 +2650,19 @@
       <c r="S27" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T27" s="42" t="s">
+      <c r="T27" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="U27" s="42" t="s">
+      <c r="U27" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="V27" s="42" t="s">
+      <c r="V27" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="W27" s="42" t="s">
+      <c r="W27" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="X27" s="42" t="s">
+      <c r="X27" s="38" t="s">
         <v>36</v>
       </c>
       <c r="Y27" s="5"/>
@@ -2719,19 +2719,19 @@
       <c r="S28" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="T28" s="42" t="s">
+      <c r="T28" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="U28" s="42" t="s">
+      <c r="U28" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="V28" s="42" t="s">
+      <c r="V28" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="W28" s="42" t="s">
+      <c r="W28" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="X28" s="42" t="s">
+      <c r="X28" s="38" t="s">
         <v>41</v>
       </c>
       <c r="Y28" s="5"/>
@@ -2788,19 +2788,19 @@
       <c r="S29" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="T29" s="42" t="s">
+      <c r="T29" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="U29" s="42" t="s">
+      <c r="U29" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="V29" s="42" t="s">
+      <c r="V29" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="W29" s="42" t="s">
+      <c r="W29" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="X29" s="42" t="s">
+      <c r="X29" s="38" t="s">
         <v>42</v>
       </c>
       <c r="Y29" s="5"/>
@@ -2857,19 +2857,19 @@
       <c r="S30" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="T30" s="42" t="s">
+      <c r="T30" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="U30" s="42" t="s">
+      <c r="U30" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="V30" s="42" t="s">
+      <c r="V30" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="W30" s="42" t="s">
+      <c r="W30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="X30" s="42" t="s">
+      <c r="X30" s="38" t="s">
         <v>43</v>
       </c>
       <c r="Y30" s="5"/>
@@ -2923,22 +2923,22 @@
       </c>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
-      <c r="S31" s="43" t="s">
+      <c r="S31" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="T31" s="44" t="s">
+      <c r="T31" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="U31" s="44" t="s">
+      <c r="U31" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="V31" s="44" t="s">
+      <c r="V31" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="W31" s="44" t="s">
+      <c r="W31" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="X31" s="44" t="s">
+      <c r="X31" s="40" t="s">
         <v>44</v>
       </c>
       <c r="Y31" s="5"/>
@@ -2975,22 +2975,22 @@
       <c r="AI32" s="5"/>
     </row>
     <row r="33" spans="1:35" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="I33" s="38" t="s">
+      <c r="B33" s="58"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="I33" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
@@ -3013,21 +3013,21 @@
     </row>
     <row r="34" spans="1:35" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
-      <c r="B34" s="39" t="s">
+      <c r="B34" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="59"/>
       <c r="I34" s="13"/>
-      <c r="J34" s="39" t="s">
+      <c r="J34" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="40"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="59"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="5"/>
       <c r="S34" s="5" t="s">
@@ -3167,7 +3167,7 @@
         <v>$T$27</v>
       </c>
       <c r="U36" s="10" t="str">
-        <f t="shared" ref="U36:U48" si="13">ADDRESS(MATCH($S36,$U$26:$U$31,0) + 25, 21)</f>
+        <f t="shared" ref="U36:U44" si="13">ADDRESS(MATCH($S36,$U$26:$U$31,0) + 25, 21)</f>
         <v>$U$26</v>
       </c>
       <c r="V36" s="10"/>
@@ -3577,7 +3577,7 @@
         <v>$W$27</v>
       </c>
       <c r="X42" s="10" t="str">
-        <f t="shared" ref="X36:X48" si="18">ADDRESS(MATCH($S42,$X$26:$X$31,0) + 25, 24)</f>
+        <f t="shared" ref="X42:X48" si="18">ADDRESS(MATCH($S42,$X$26:$X$31,0) + 25, 24)</f>
         <v>$X$26</v>
       </c>
       <c r="Y42" s="5"/>
@@ -3910,32 +3910,32 @@
       </c>
     </row>
     <row r="53" spans="1:24" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="51" t="s">
+      <c r="A53" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="52"/>
-      <c r="C53" s="52"/>
-      <c r="D53" s="52"/>
-      <c r="E53" s="52"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="57" t="s">
+      <c r="B53" s="56"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="H53" s="57" t="s">
+      <c r="H53" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="I53" s="51" t="s">
+      <c r="I53" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="J53" s="52"/>
-      <c r="K53" s="52"/>
-      <c r="L53" s="52"/>
-      <c r="M53" s="52"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="57" t="s">
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="57"/>
+      <c r="O53" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="P53" s="57" t="s">
+      <c r="P53" s="50" t="s">
         <v>81</v>
       </c>
       <c r="S53" s="5" t="s">
@@ -3946,38 +3946,38 @@
       </c>
     </row>
     <row r="54" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="46" cm="1">
+      <c r="B54" s="42" cm="1">
         <f t="array" aca="1" ref="B54" ca="1">OFFSET(INDIRECT(T51), -22,-18)</f>
         <v>103.30378643453901</v>
       </c>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="55">
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="48">
         <f ca="1">AVERAGE(B54:F54)</f>
         <v>103.30378643453901</v>
       </c>
-      <c r="H54" s="54"/>
-      <c r="I54" s="45" t="s">
+      <c r="H54" s="47"/>
+      <c r="I54" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="J54" s="46" cm="1">
+      <c r="J54" s="42" cm="1">
         <f t="array" aca="1" ref="J54" ca="1">OFFSET(INDIRECT(T51), -22,-10)</f>
         <v>2946.1254700178702</v>
       </c>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="47"/>
-      <c r="O54" s="59">
+      <c r="K54" s="42"/>
+      <c r="L54" s="42"/>
+      <c r="M54" s="42"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="52">
         <f ca="1">AVERAGE(J54:N54)</f>
         <v>2946.1254700178702</v>
       </c>
-      <c r="P54" s="54"/>
+      <c r="P54" s="47"/>
       <c r="S54" s="5" t="s">
         <v>33</v>
       </c>
@@ -3992,48 +3992,48 @@
       </c>
     </row>
     <row r="55" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="46" cm="1">
+      <c r="B55" s="42" cm="1">
         <f t="array" aca="1" ref="B55" ca="1">OFFSET(INDIRECT(T52), -22,-18)</f>
         <v>110.295288662046</v>
       </c>
-      <c r="C55" s="46" cm="1">
+      <c r="C55" s="42" cm="1">
         <f t="array" aca="1" ref="C55" ca="1">OFFSET(INDIRECT(U52), -22,-18)</f>
         <v>97.726402420994006</v>
       </c>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="55">
+      <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="F55" s="42"/>
+      <c r="G55" s="48">
         <f t="shared" ref="G55:G67" ca="1" si="19">AVERAGE(B55:F55)</f>
         <v>104.01084554152001</v>
       </c>
-      <c r="H55" s="55">
-        <f t="shared" ref="H55:H67" ca="1" si="20">_xlfn.STDEV.S(B55:F55)</f>
+      <c r="H55" s="48">
+        <f ca="1">_xlfn.STDEV.S(B55:F55)</f>
         <v>8.8875446930101631</v>
       </c>
-      <c r="I55" s="45" t="s">
+      <c r="I55" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="J55" s="46" cm="1">
+      <c r="J55" s="42" cm="1">
         <f t="array" aca="1" ref="J55" ca="1">OFFSET(INDIRECT(T52), -22,-10)</f>
         <v>3168.1744314970001</v>
       </c>
-      <c r="K55" s="46" cm="1">
+      <c r="K55" s="42" cm="1">
         <f t="array" aca="1" ref="K55" ca="1">OFFSET(INDIRECT(U52), -22,-10)</f>
         <v>2979.7594087393099</v>
       </c>
-      <c r="L55" s="46"/>
-      <c r="M55" s="46"/>
-      <c r="N55" s="47"/>
-      <c r="O55" s="58">
-        <f t="shared" ref="O55:O67" ca="1" si="21">AVERAGE(J55:N55)</f>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="51">
+        <f t="shared" ref="O55:O67" ca="1" si="20">AVERAGE(J55:N55)</f>
         <v>3073.966920118155</v>
       </c>
-      <c r="P55" s="55">
-        <f t="shared" ref="P55:P67" ca="1" si="22">_xlfn.STDEV.S(J55:N55)</f>
+      <c r="P55" s="48">
+        <f t="shared" ref="P55:P66" ca="1" si="21">_xlfn.STDEV.S(J55:N55)</f>
         <v>133.22954026938038</v>
       </c>
       <c r="S55" s="5" t="s">
@@ -4044,38 +4044,38 @@
       </c>
     </row>
     <row r="56" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="46" cm="1">
+      <c r="B56" s="42" cm="1">
         <f t="array" aca="1" ref="B56" ca="1">OFFSET(INDIRECT(T53), -22,-18)</f>
         <v>128.20496596054301</v>
       </c>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
-      <c r="F56" s="46"/>
-      <c r="G56" s="55">
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="F56" s="42"/>
+      <c r="G56" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>128.20496596054301</v>
       </c>
-      <c r="H56" s="55"/>
-      <c r="I56" s="45" t="s">
+      <c r="H56" s="48"/>
+      <c r="I56" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="J56" s="46" cm="1">
+      <c r="J56" s="42" cm="1">
         <f t="array" aca="1" ref="J56" ca="1">OFFSET(INDIRECT(T53), -22,-10)</f>
         <v>3743.62111203829</v>
       </c>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="47"/>
-      <c r="O56" s="58">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K56" s="42"/>
+      <c r="L56" s="42"/>
+      <c r="M56" s="42"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="51">
+        <f t="shared" ca="1" si="20"/>
         <v>3743.62111203829</v>
       </c>
-      <c r="P56" s="55"/>
+      <c r="P56" s="48"/>
       <c r="S56" s="5" t="s">
         <v>34</v>
       </c>
@@ -4093,54 +4093,54 @@
       </c>
     </row>
     <row r="57" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="46" cm="1">
+      <c r="B57" s="42" cm="1">
         <f t="array" aca="1" ref="B57" ca="1">OFFSET(INDIRECT(T54), -22,-18)</f>
         <v>152.12652616182299</v>
       </c>
-      <c r="C57" s="46" cm="1">
+      <c r="C57" s="42" cm="1">
         <f t="array" aca="1" ref="C57" ca="1">OFFSET(INDIRECT(U54), -22,-18)</f>
         <v>85.012633346330404</v>
       </c>
-      <c r="D57" s="46" cm="1">
+      <c r="D57" s="42" cm="1">
         <f t="array" aca="1" ref="D57" ca="1">OFFSET(INDIRECT(V54), -22,-18)</f>
         <v>138.87799154853599</v>
       </c>
-      <c r="E57" s="46"/>
-      <c r="F57" s="46"/>
-      <c r="G57" s="55">
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>125.33905035222979</v>
       </c>
-      <c r="H57" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H57" s="48">
+        <f ca="1">_xlfn.STDEV.S(B57:F57)</f>
         <v>35.546390094496722</v>
       </c>
-      <c r="I57" s="45" t="s">
+      <c r="I57" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="J57" s="46" cm="1">
+      <c r="J57" s="42" cm="1">
         <f t="array" aca="1" ref="J57" ca="1">OFFSET(INDIRECT(T54), -22,-10)</f>
         <v>4501.7049593007996</v>
       </c>
-      <c r="K57" s="46" cm="1">
+      <c r="K57" s="42" cm="1">
         <f t="array" aca="1" ref="K57" ca="1">OFFSET(INDIRECT(U54), -22,-10)</f>
         <v>2413.0167329626402</v>
       </c>
-      <c r="L57" s="46" cm="1">
+      <c r="L57" s="42" cm="1">
         <f t="array" aca="1" ref="L57" ca="1">OFFSET(INDIRECT(V54), -22,-10)</f>
         <v>4299.5268815057798</v>
       </c>
-      <c r="M57" s="46"/>
-      <c r="N57" s="47"/>
-      <c r="O57" s="58">
+      <c r="M57" s="42"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>3738.0828579230729</v>
+      </c>
+      <c r="P57" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>3738.0828579230729</v>
-      </c>
-      <c r="P57" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>1151.984882897111</v>
       </c>
       <c r="S57" s="5" t="s">
@@ -4151,38 +4151,38 @@
       </c>
     </row>
     <row r="58" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B58" s="46" cm="1">
+      <c r="B58" s="42" cm="1">
         <f t="array" aca="1" ref="B58" ca="1">OFFSET(INDIRECT(T55), -22,-18)</f>
         <v>84.923331060488096</v>
       </c>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
-      <c r="E58" s="46"/>
-      <c r="F58" s="46"/>
-      <c r="G58" s="55">
+      <c r="C58" s="42"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>84.923331060488096</v>
       </c>
-      <c r="H58" s="55"/>
-      <c r="I58" s="45" t="s">
+      <c r="H58" s="48"/>
+      <c r="I58" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="J58" s="46" cm="1">
+      <c r="J58" s="42" cm="1">
         <f t="array" aca="1" ref="J58" ca="1">OFFSET(INDIRECT(T55), -22,-10)</f>
         <v>2364.2307007107902</v>
       </c>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="47"/>
-      <c r="O58" s="58">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K58" s="42"/>
+      <c r="L58" s="42"/>
+      <c r="M58" s="42"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="51">
+        <f t="shared" ca="1" si="20"/>
         <v>2364.2307007107902</v>
       </c>
-      <c r="P58" s="55"/>
+      <c r="P58" s="48"/>
       <c r="S58" s="5" t="s">
         <v>35</v>
       </c>
@@ -4203,60 +4203,60 @@
       </c>
     </row>
     <row r="59" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B59" s="46" cm="1">
+      <c r="B59" s="42" cm="1">
         <f t="array" aca="1" ref="B59" ca="1">OFFSET(INDIRECT(T56), -22,-18)</f>
         <v>199.55653595381801</v>
       </c>
-      <c r="C59" s="46" cm="1">
+      <c r="C59" s="42" cm="1">
         <f t="array" aca="1" ref="C59" ca="1">OFFSET(INDIRECT(U56), -22,-18)</f>
         <v>95.993434196655599</v>
       </c>
-      <c r="D59" s="46" cm="1">
+      <c r="D59" s="42" cm="1">
         <f t="array" aca="1" ref="D59" ca="1">OFFSET(INDIRECT(V56), -22,-18)</f>
         <v>145.52280163016201</v>
       </c>
-      <c r="E59" s="46" cm="1">
+      <c r="E59" s="42" cm="1">
         <f t="array" aca="1" ref="E59" ca="1">OFFSET(INDIRECT(W56), -22,-18)</f>
         <v>172.03332083348599</v>
       </c>
-      <c r="F59" s="46"/>
-      <c r="G59" s="55">
+      <c r="F59" s="42"/>
+      <c r="G59" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>153.27652315353041</v>
       </c>
-      <c r="H59" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H59" s="48">
+        <f t="shared" ref="H55:H66" ca="1" si="22">_xlfn.STDEV.S(B59:F59)</f>
         <v>44.102643616548079</v>
       </c>
-      <c r="I59" s="45" t="s">
+      <c r="I59" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="J59" s="46" cm="1">
+      <c r="J59" s="42" cm="1">
         <f t="array" aca="1" ref="J59" ca="1">OFFSET(INDIRECT(T56), -22,-10)</f>
         <v>5989.3025805570796</v>
       </c>
-      <c r="K59" s="46" cm="1">
+      <c r="K59" s="42" cm="1">
         <f t="array" aca="1" ref="K59" ca="1">OFFSET(INDIRECT(U56), -22,-10)</f>
         <v>2712.6220681065702</v>
       </c>
-      <c r="L59" s="46" cm="1">
+      <c r="L59" s="42" cm="1">
         <f t="array" aca="1" ref="L59" ca="1">OFFSET(INDIRECT(V56), -22,-10)</f>
         <v>4436.6622230803396</v>
       </c>
-      <c r="M59" s="46" cm="1">
+      <c r="M59" s="42" cm="1">
         <f t="array" aca="1" ref="M59" ca="1">OFFSET(INDIRECT(W56), -22,-10)</f>
         <v>5319.3879846218697</v>
       </c>
-      <c r="N59" s="47"/>
-      <c r="O59" s="58">
+      <c r="N59" s="43"/>
+      <c r="O59" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>4614.4937140914644</v>
+      </c>
+      <c r="P59" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>4614.4937140914644</v>
-      </c>
-      <c r="P59" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>1418.4163879641269</v>
       </c>
       <c r="S59" s="5" t="s">
@@ -4267,38 +4267,38 @@
       </c>
     </row>
     <row r="60" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="46" cm="1">
+      <c r="B60" s="42" cm="1">
         <f t="array" aca="1" ref="B60" ca="1">OFFSET(INDIRECT(T57), -22,-18)</f>
         <v>145.87366553946899</v>
       </c>
-      <c r="C60" s="46"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="55">
+      <c r="C60" s="42"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>145.87366553946899</v>
       </c>
-      <c r="H60" s="55"/>
-      <c r="I60" s="45" t="s">
+      <c r="H60" s="48"/>
+      <c r="I60" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="J60" s="46" cm="1">
+      <c r="J60" s="42" cm="1">
         <f t="array" aca="1" ref="J60" ca="1">OFFSET(INDIRECT(T57), -22,-10)</f>
         <v>4410.2484623073497</v>
       </c>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="46"/>
-      <c r="N60" s="47"/>
-      <c r="O60" s="58">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="42"/>
+      <c r="M60" s="42"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="51">
+        <f t="shared" ca="1" si="20"/>
         <v>4410.2484623073497</v>
       </c>
-      <c r="P60" s="55"/>
+      <c r="P60" s="48"/>
       <c r="S60" s="5" t="s">
         <v>36</v>
       </c>
@@ -4316,66 +4316,66 @@
       </c>
     </row>
     <row r="61" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="45" t="s">
+      <c r="A61" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="B61" s="46" cm="1">
+      <c r="B61" s="42" cm="1">
         <f t="array" aca="1" ref="B61" ca="1">OFFSET(INDIRECT(T58), -22,-18)</f>
         <v>220.05977047235601</v>
       </c>
-      <c r="C61" s="46" cm="1">
+      <c r="C61" s="42" cm="1">
         <f t="array" aca="1" ref="C61" ca="1">OFFSET(INDIRECT(U58), -22,-18)</f>
         <v>135.92960294240399</v>
       </c>
-      <c r="D61" s="46" cm="1">
+      <c r="D61" s="42" cm="1">
         <f t="array" aca="1" ref="D61" ca="1">OFFSET(INDIRECT(V58), -22,-18)</f>
         <v>142.158969876388</v>
       </c>
-      <c r="E61" s="46" cm="1">
+      <c r="E61" s="42" cm="1">
         <f t="array" aca="1" ref="E61" ca="1">OFFSET(INDIRECT(W58), -22,-18)</f>
         <v>194.42156250270099</v>
       </c>
-      <c r="F61" s="46" cm="1">
+      <c r="F61" s="42" cm="1">
         <f t="array" aca="1" ref="F61" ca="1">OFFSET(INDIRECT(X58), -22,-18)</f>
         <v>183.02148279631899</v>
       </c>
-      <c r="G61" s="55">
+      <c r="G61" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>175.1182777180336</v>
       </c>
-      <c r="H61" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H61" s="48">
+        <f t="shared" ca="1" si="22"/>
         <v>35.626126049026944</v>
       </c>
-      <c r="I61" s="45" t="s">
+      <c r="I61" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="J61" s="46" cm="1">
+      <c r="J61" s="42" cm="1">
         <f t="array" aca="1" ref="J61" ca="1">OFFSET(INDIRECT(T58), -22,-10)</f>
         <v>6632.3182166696197</v>
       </c>
-      <c r="K61" s="46" cm="1">
+      <c r="K61" s="42" cm="1">
         <f t="array" aca="1" ref="K61" ca="1">OFFSET(INDIRECT(U58), -22,-10)</f>
         <v>3997.3977459525099</v>
       </c>
-      <c r="L61" s="46" cm="1">
+      <c r="L61" s="42" cm="1">
         <f t="array" aca="1" ref="L61" ca="1">OFFSET(INDIRECT(V58), -22,-10)</f>
         <v>4257.6395901932701</v>
       </c>
-      <c r="M61" s="46" cm="1">
+      <c r="M61" s="42" cm="1">
         <f t="array" aca="1" ref="M61" ca="1">OFFSET(INDIRECT(W58), -22,-10)</f>
         <v>5951.2040552038097</v>
       </c>
-      <c r="N61" s="47" cm="1">
+      <c r="N61" s="43" cm="1">
         <f t="array" aca="1" ref="N61" ca="1">OFFSET(INDIRECT(X58), -22,-10)</f>
         <v>5668.9924665783101</v>
       </c>
-      <c r="O61" s="58">
+      <c r="O61" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>5301.510414919504</v>
+      </c>
+      <c r="P61" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>5301.510414919504</v>
-      </c>
-      <c r="P61" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>1131.2128935119881</v>
       </c>
       <c r="S61" s="5" t="s">
@@ -4386,38 +4386,38 @@
       </c>
     </row>
     <row r="62" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="45" t="s">
+      <c r="A62" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="46" cm="1">
+      <c r="B62" s="42" cm="1">
         <f t="array" aca="1" ref="B62" ca="1">OFFSET(INDIRECT(T59), -22,-18)</f>
         <v>213.21970815858401</v>
       </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="55">
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>213.21970815858401</v>
       </c>
-      <c r="H62" s="55"/>
-      <c r="I62" s="45" t="s">
+      <c r="H62" s="48"/>
+      <c r="I62" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="J62" s="46" cm="1">
+      <c r="J62" s="42" cm="1">
         <f t="array" aca="1" ref="J62" ca="1">OFFSET(INDIRECT(T59), -22,-10)</f>
         <v>6504.1082488594202</v>
       </c>
-      <c r="K62" s="46"/>
-      <c r="L62" s="46"/>
-      <c r="M62" s="46"/>
-      <c r="N62" s="47"/>
-      <c r="O62" s="58">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K62" s="42"/>
+      <c r="L62" s="42"/>
+      <c r="M62" s="42"/>
+      <c r="N62" s="43"/>
+      <c r="O62" s="51">
+        <f t="shared" ca="1" si="20"/>
         <v>6504.1082488594202</v>
       </c>
-      <c r="P62" s="55"/>
+      <c r="P62" s="48"/>
       <c r="S62" s="5" t="s">
         <v>42</v>
       </c>
@@ -4432,60 +4432,60 @@
       </c>
     </row>
     <row r="63" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="46" cm="1">
+      <c r="B63" s="42" cm="1">
         <f t="array" aca="1" ref="B63" ca="1">OFFSET(INDIRECT(T60), -22,-18)</f>
         <v>167.208983842083</v>
       </c>
-      <c r="C63" s="46" cm="1">
+      <c r="C63" s="42" cm="1">
         <f t="array" aca="1" ref="C63" ca="1">OFFSET(INDIRECT(U60), -22,-18)</f>
         <v>139.15709922839901</v>
       </c>
-      <c r="D63" s="46" cm="1">
+      <c r="D63" s="42" cm="1">
         <f t="array" aca="1" ref="D63" ca="1">OFFSET(INDIRECT(V60), -22,-18)</f>
         <v>233.35858507467401</v>
       </c>
-      <c r="E63" s="46" cm="1">
+      <c r="E63" s="42" cm="1">
         <f t="array" aca="1" ref="E63" ca="1">OFFSET(INDIRECT(W60), -22,-18)</f>
         <v>204.96386973052199</v>
       </c>
-      <c r="F63" s="46"/>
-      <c r="G63" s="55">
+      <c r="F63" s="42"/>
+      <c r="G63" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>186.1721344689195</v>
       </c>
-      <c r="H63" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H63" s="48">
+        <f t="shared" ca="1" si="22"/>
         <v>41.431489856850718</v>
       </c>
-      <c r="I63" s="45" t="s">
+      <c r="I63" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="J63" s="46" cm="1">
+      <c r="J63" s="42" cm="1">
         <f t="array" aca="1" ref="J63" ca="1">OFFSET(INDIRECT(T60), -22,-10)</f>
         <v>4988.9862664472603</v>
       </c>
-      <c r="K63" s="46" cm="1">
+      <c r="K63" s="42" cm="1">
         <f t="array" aca="1" ref="K63" ca="1">OFFSET(INDIRECT(U60), -22,-10)</f>
         <v>4094.43301523434</v>
       </c>
-      <c r="L63" s="46" cm="1">
+      <c r="L63" s="42" cm="1">
         <f t="array" aca="1" ref="L63" ca="1">OFFSET(INDIRECT(V60), -22,-10)</f>
         <v>7102.74596657652</v>
       </c>
-      <c r="M63" s="46" cm="1">
+      <c r="M63" s="42" cm="1">
         <f t="array" aca="1" ref="M63" ca="1">OFFSET(INDIRECT(W60), -22,-10)</f>
         <v>6270.4202619384296</v>
       </c>
-      <c r="N63" s="47"/>
-      <c r="O63" s="58">
+      <c r="N63" s="43"/>
+      <c r="O63" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>5614.1463775491375</v>
+      </c>
+      <c r="P63" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>5614.1463775491375</v>
-      </c>
-      <c r="P63" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>1335.0378291637755</v>
       </c>
       <c r="S63" s="5" t="s">
@@ -4499,38 +4499,38 @@
       </c>
     </row>
     <row r="64" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="45" t="s">
+      <c r="A64" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="46" cm="1">
+      <c r="B64" s="42" cm="1">
         <f t="array" aca="1" ref="B64" ca="1">OFFSET(INDIRECT(T61), -22,-18)</f>
         <v>224.70980127730999</v>
       </c>
-      <c r="C64" s="46"/>
-      <c r="D64" s="46"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="55">
+      <c r="C64" s="42"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>224.70980127730999</v>
       </c>
-      <c r="H64" s="55"/>
-      <c r="I64" s="45" t="s">
+      <c r="H64" s="48"/>
+      <c r="I64" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="J64" s="46" cm="1">
+      <c r="J64" s="42" cm="1">
         <f t="array" aca="1" ref="J64" ca="1">OFFSET(INDIRECT(T61), -22,-10)</f>
         <v>6838.06180030223</v>
       </c>
-      <c r="K64" s="46"/>
-      <c r="L64" s="46"/>
-      <c r="M64" s="46"/>
-      <c r="N64" s="47"/>
-      <c r="O64" s="58">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K64" s="42"/>
+      <c r="L64" s="42"/>
+      <c r="M64" s="42"/>
+      <c r="N64" s="43"/>
+      <c r="O64" s="51">
+        <f t="shared" ca="1" si="20"/>
         <v>6838.06180030223</v>
       </c>
-      <c r="P64" s="55"/>
+      <c r="P64" s="48"/>
       <c r="S64" s="5" t="s">
         <v>44</v>
       </c>
@@ -4539,151 +4539,140 @@
       </c>
     </row>
     <row r="65" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="45" t="s">
+      <c r="A65" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="46" cm="1">
+      <c r="B65" s="42" cm="1">
         <f t="array" aca="1" ref="B65" ca="1">OFFSET(INDIRECT(T62), -22,-18)</f>
         <v>165.040468203405</v>
       </c>
-      <c r="C65" s="46" cm="1">
+      <c r="C65" s="42" cm="1">
         <f t="array" aca="1" ref="C65" ca="1">OFFSET(INDIRECT(U62), -22,-18)</f>
         <v>274.44411939937203</v>
       </c>
-      <c r="D65" s="46" cm="1">
+      <c r="D65" s="42" cm="1">
         <f t="array" aca="1" ref="D65" ca="1">OFFSET(INDIRECT(V62), -22,-18)</f>
         <v>247.39652666738499</v>
       </c>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="55">
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>228.96037142338733</v>
       </c>
-      <c r="H65" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H65" s="48">
+        <f t="shared" ca="1" si="22"/>
         <v>56.984283700752016</v>
       </c>
-      <c r="I65" s="45" t="s">
+      <c r="I65" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="J65" s="46" cm="1">
+      <c r="J65" s="42" cm="1">
         <f t="array" aca="1" ref="J65" ca="1">OFFSET(INDIRECT(T62), -22,-10)</f>
         <v>4882.4302342429601</v>
       </c>
-      <c r="K65" s="46" cm="1">
+      <c r="K65" s="42" cm="1">
         <f t="array" aca="1" ref="K65" ca="1">OFFSET(INDIRECT(U62), -22,-10)</f>
         <v>8330.9895359191596</v>
       </c>
-      <c r="L65" s="46" cm="1">
+      <c r="L65" s="42" cm="1">
         <f t="array" aca="1" ref="L65" ca="1">OFFSET(INDIRECT(V62), -22,-10)</f>
         <v>7486.9981927108201</v>
       </c>
-      <c r="M65" s="46"/>
-      <c r="N65" s="47"/>
-      <c r="O65" s="58">
+      <c r="M65" s="42"/>
+      <c r="N65" s="43"/>
+      <c r="O65" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>6900.1393209576463</v>
+      </c>
+      <c r="P65" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>6900.1393209576463</v>
-      </c>
-      <c r="P65" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>1797.6214328414419</v>
       </c>
       <c r="S65" s="5"/>
     </row>
     <row r="66" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="45" t="s">
+      <c r="A66" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="B66" s="46" cm="1">
+      <c r="B66" s="42" cm="1">
         <f t="array" aca="1" ref="B66" ca="1">OFFSET(INDIRECT(T63), -22,-18)</f>
         <v>316.66403127578002</v>
       </c>
-      <c r="C66" s="46" cm="1">
+      <c r="C66" s="42" cm="1">
         <f t="array" aca="1" ref="C66" ca="1">OFFSET(INDIRECT(U63), -22,-18)</f>
         <v>370.91765882374301</v>
       </c>
-      <c r="D66" s="46"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="55">
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="48">
         <f t="shared" ca="1" si="19"/>
         <v>343.79084504976151</v>
       </c>
-      <c r="H66" s="55">
-        <f t="shared" ca="1" si="20"/>
+      <c r="H66" s="48">
+        <f t="shared" ca="1" si="22"/>
         <v>38.363107943133912</v>
       </c>
-      <c r="I66" s="45" t="s">
+      <c r="I66" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="J66" s="46" cm="1">
+      <c r="J66" s="42" cm="1">
         <f t="array" aca="1" ref="J66" ca="1">OFFSET(INDIRECT(T63), -22,-10)</f>
         <v>9596.1134963183595</v>
       </c>
-      <c r="K66" s="46" cm="1">
+      <c r="K66" s="42" cm="1">
         <f t="array" aca="1" ref="K66" ca="1">OFFSET(INDIRECT(U63), -22,-10)</f>
         <v>8288.3137383518606</v>
       </c>
-      <c r="L66" s="46"/>
-      <c r="M66" s="46"/>
-      <c r="N66" s="47"/>
-      <c r="O66" s="58">
+      <c r="L66" s="42"/>
+      <c r="M66" s="42"/>
+      <c r="N66" s="43"/>
+      <c r="O66" s="51">
+        <f t="shared" ca="1" si="20"/>
+        <v>8942.21361733511</v>
+      </c>
+      <c r="P66" s="48">
         <f t="shared" ca="1" si="21"/>
-        <v>8942.21361733511</v>
-      </c>
-      <c r="P66" s="55">
-        <f t="shared" ca="1" si="22"/>
         <v>924.75407729223696</v>
       </c>
     </row>
     <row r="67" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="48" t="s">
+      <c r="A67" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="49" cm="1">
+      <c r="B67" s="45" cm="1">
         <f t="array" aca="1" ref="B67" ca="1">OFFSET(INDIRECT(T64), -22,-18)</f>
         <v>473.89533622516501</v>
       </c>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="56">
+      <c r="C67" s="45"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="49">
         <f t="shared" ca="1" si="19"/>
         <v>473.89533622516501</v>
       </c>
-      <c r="H67" s="56"/>
-      <c r="I67" s="48" t="s">
+      <c r="H67" s="49"/>
+      <c r="I67" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="J67" s="49" cm="1">
+      <c r="J67" s="45" cm="1">
         <f t="array" aca="1" ref="J67" ca="1">OFFSET(INDIRECT(T64), -22,-10)</f>
         <v>8747.3580818581395</v>
       </c>
-      <c r="K67" s="49"/>
-      <c r="L67" s="49"/>
-      <c r="M67" s="49"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="60">
-        <f t="shared" ca="1" si="21"/>
+      <c r="K67" s="45"/>
+      <c r="L67" s="45"/>
+      <c r="M67" s="45"/>
+      <c r="N67" s="46"/>
+      <c r="O67" s="53">
+        <f t="shared" ca="1" si="20"/>
         <v>8747.3580818581395</v>
       </c>
-      <c r="P67" s="56"/>
+      <c r="P67" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="T24:X24"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="I53:N53"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="I33:N33"/>
-    <mergeCell ref="A33:F33"/>
     <mergeCell ref="S1:Y1"/>
     <mergeCell ref="T2:Y2"/>
     <mergeCell ref="S13:Y13"/>
@@ -4696,6 +4685,17 @@
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="T24:X24"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="I53:N53"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="A33:F33"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F9">
     <cfRule type="colorScale" priority="32">
@@ -4757,6 +4757,42 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B54:F67">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G54:G67">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54:H67">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="J4:N9">
     <cfRule type="colorScale" priority="27">
       <colorScale>
@@ -4805,6 +4841,54 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J54:N67">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O54:O67">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P54:P67">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T35:T48">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="T4:X9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
@@ -4819,18 +4903,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="T16:X21">
     <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T35:T48">
-    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4889,78 +4961,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:F67">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J54:N67">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O54:O67">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54:G67">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H54:H67">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P54:P67">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="T10:X10 T22:X22" formulaRange="1"/>

</xml_diff>